<commit_message>
Major update. Changes from the HIDA research stay at HMGU.
</commit_message>
<xml_diff>
--- a/docs/overview.xlsx
+++ b/docs/overview.xlsx
@@ -66,10 +66,7 @@
     <t>patient</t>
   </si>
   <si>
-    <t>dpso_value</t>
-  </si>
-  <si>
-    <t>dpso_type</t>
+    <t>dpso</t>
   </si>
   <si>
     <r>
@@ -112,9 +109,6 @@
     <t>Neph_X1</t>
   </si>
   <si>
-    <t>d</t>
-  </si>
-  <si>
     <t xml:space="preserve">COVID-19 ARDS</t>
   </si>
   <si>
@@ -130,7 +124,7 @@
     <t>C19-CB-0062</t>
   </si>
   <si>
-    <t>Initial</t>
+    <t>A</t>
   </si>
   <si>
     <t>BAL_3-6</t>
@@ -190,6 +184,9 @@
     <t>C19-CB-0198</t>
   </si>
   <si>
+    <t>C</t>
+  </si>
+  <si>
     <t>200701_A00643_0061_AHMNCCDRXX</t>
   </si>
   <si>
@@ -241,7 +238,7 @@
     <t>C19-CB-0660</t>
   </si>
   <si>
-    <t>Second</t>
+    <t>B</t>
   </si>
   <si>
     <t>210215_A00643_0181_BHVFHHDSXY</t>
@@ -317,6 +314,9 @@
   </si>
   <si>
     <t>Recovery</t>
+  </si>
+  <si>
+    <t>221014_A00643_0567_AHYMN3DSX3</t>
   </si>
   <si>
     <t>C19-CB-0914</t>
@@ -529,7 +529,7 @@
     <xf fontId="2" fillId="3" borderId="0" numFmtId="0" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="0"/>
     <xf fontId="3" fillId="4" borderId="0" numFmtId="0" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="16">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0">
       <protection hidden="0" locked="1"/>
@@ -540,6 +540,8 @@
     <xf fontId="0" fillId="5" borderId="0" numFmtId="0" xfId="0" applyFill="1"/>
     <xf fontId="0" fillId="5" borderId="0" numFmtId="0" xfId="0" applyFill="1"/>
     <xf fontId="0" fillId="6" borderId="0" numFmtId="0" xfId="0" applyFill="1"/>
+    <xf fontId="0" fillId="6" borderId="0" numFmtId="0" xfId="0" applyFill="1"/>
+    <xf fontId="0" fillId="7" borderId="0" numFmtId="0" xfId="0" applyFill="1"/>
     <xf fontId="0" fillId="7" borderId="0" numFmtId="0" xfId="0" applyFill="1"/>
     <xf fontId="0" fillId="8" borderId="0" numFmtId="0" xfId="0" applyFill="1"/>
     <xf fontId="0" fillId="8" borderId="0" numFmtId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -547,6 +549,7 @@
     </xf>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="0" fillId="9" borderId="0" numFmtId="0" xfId="0" applyFill="1"/>
+    <xf fontId="0" fillId="10" borderId="0" numFmtId="0" xfId="0" applyFill="1"/>
     <xf fontId="0" fillId="10" borderId="0" numFmtId="0" xfId="0" applyFill="1"/>
     <xf fontId="1" fillId="2" borderId="0" numFmtId="0" xfId="1" applyFont="1" applyFill="1">
       <protection hidden="0" locked="1"/>
@@ -1061,7 +1064,7 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
   <sheetViews>
-    <sheetView zoomScale="100" workbookViewId="0">
+    <sheetView topLeftCell="A22" zoomScale="100" workbookViewId="0">
       <selection activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -1074,11 +1077,12 @@
     <col customWidth="1" min="5" max="5" width="11.57421875"/>
     <col customWidth="1" min="6" max="6" width="14.140625"/>
     <col customWidth="1" min="7" max="7" width="11.00390625"/>
-    <col customWidth="1" min="8" max="8" width="10.57421875"/>
-    <col customWidth="1" min="9" max="10" width="17.8515625"/>
-    <col customWidth="1" min="11" max="11" width="38.28125"/>
-    <col customWidth="1" min="14" max="14" width="15.421875"/>
-    <col customWidth="1" min="15" max="15" width="4.28125"/>
+    <col customWidth="1" min="8" max="9" width="17.8515625"/>
+    <col customWidth="1" min="10" max="10" width="38.28125"/>
+    <col bestFit="1" min="11" max="11" width="10.421875"/>
+    <col bestFit="1" min="12" max="12" width="9.421875"/>
+    <col customWidth="1" min="13" max="13" width="15.421875"/>
+    <col customWidth="1" min="14" max="14" width="4.28125"/>
   </cols>
   <sheetData>
     <row r="1" ht="15">
@@ -1103,7 +1107,7 @@
       <c r="G1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
       <c r="I1" s="1" t="s">
@@ -1112,1406 +1116,1472 @@
       <c r="J1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
-        <v>10</v>
-      </c>
     </row>
     <row r="2" ht="14.25">
       <c r="A2" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B2" s="3">
         <v>1</v>
       </c>
       <c r="C2" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="E2" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="F2" s="3" t="s">
         <v>14</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>15</v>
       </c>
       <c r="G2" s="3">
         <v>14</v>
       </c>
       <c r="H2" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="I2" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="I2" s="3" t="s">
+      <c r="J2" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="J2" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="K2" s="3" t="s">
-        <v>19</v>
-      </c>
+      <c r="M2" s="1"/>
       <c r="N2" s="1"/>
       <c r="O2" s="1"/>
-      <c r="P2" s="1"/>
     </row>
     <row r="3" ht="14.25">
       <c r="A3" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B3" s="3">
         <v>2</v>
       </c>
       <c r="C3" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="D3" s="3" t="s">
-        <v>13</v>
-      </c>
       <c r="E3" s="3" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="G3" s="3">
         <v>14</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="I3" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="I3" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="J3" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="J3" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="K3" s="3" t="s">
-        <v>19</v>
-      </c>
+      <c r="M3" s="1"/>
       <c r="N3" s="1"/>
       <c r="O3" s="1"/>
-      <c r="P3" s="1"/>
     </row>
     <row r="4" ht="14.25">
       <c r="A4" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B4" s="5">
         <v>3</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D4" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="F4" s="5" t="s">
         <v>23</v>
-      </c>
-      <c r="E4" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="F4" s="5" t="s">
-        <v>25</v>
       </c>
       <c r="G4" s="5">
         <v>7</v>
       </c>
       <c r="H4" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="I4" s="5" t="s">
-        <v>17</v>
+        <v>15</v>
+      </c>
+      <c r="I4" s="6" t="s">
+        <v>20</v>
       </c>
       <c r="J4" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="K4" s="5" t="s">
-        <v>26</v>
-      </c>
+        <v>24</v>
+      </c>
+      <c r="M4" s="1"/>
       <c r="N4" s="1"/>
       <c r="O4" s="1"/>
-      <c r="P4" s="1"/>
     </row>
     <row r="5" ht="14.25">
       <c r="A5" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B5" s="5">
         <v>4</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="G5" s="5">
         <v>14</v>
       </c>
       <c r="H5" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="I5" s="5" t="s">
-        <v>17</v>
+        <v>15</v>
+      </c>
+      <c r="I5" s="6" t="s">
+        <v>20</v>
       </c>
       <c r="J5" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="K5" s="5" t="s">
-        <v>26</v>
-      </c>
+        <v>24</v>
+      </c>
+      <c r="M5" s="1"/>
       <c r="N5" s="1"/>
       <c r="O5" s="1"/>
-      <c r="P5" s="1"/>
     </row>
     <row r="6" ht="14.25">
       <c r="A6" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B6" s="5">
         <v>5</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="G6" s="5">
         <v>25</v>
       </c>
       <c r="H6" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="I6" s="5" t="s">
-        <v>17</v>
+        <v>15</v>
+      </c>
+      <c r="I6" s="6" t="s">
+        <v>20</v>
       </c>
       <c r="J6" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="K6" s="5" t="s">
-        <v>26</v>
-      </c>
+        <v>24</v>
+      </c>
+      <c r="M6" s="1"/>
       <c r="N6" s="1"/>
       <c r="O6" s="1"/>
-      <c r="P6" s="1"/>
     </row>
     <row r="7" ht="14.25">
       <c r="A7" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B7" s="5">
         <v>6</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="G7" s="5">
         <v>7</v>
       </c>
       <c r="H7" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="I7" s="5" t="s">
-        <v>17</v>
+        <v>15</v>
+      </c>
+      <c r="I7" s="6" t="s">
+        <v>20</v>
       </c>
       <c r="J7" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="K7" s="5" t="s">
-        <v>26</v>
-      </c>
+        <v>24</v>
+      </c>
+      <c r="M7" s="1"/>
       <c r="N7" s="1"/>
       <c r="O7" s="1"/>
-      <c r="P7" s="1"/>
     </row>
     <row r="8" ht="14.25">
-      <c r="A8" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="B8" s="6">
+      <c r="A8" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8" s="7">
         <v>7</v>
       </c>
-      <c r="C8" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="D8" s="6" t="s">
+      <c r="C8" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="D8" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="E8" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="F8" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="E8" s="6" t="s">
+      <c r="G8" s="7">
+        <v>25</v>
+      </c>
+      <c r="H8" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="I8" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="J8" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="F8" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="G8" s="6">
-        <v>25</v>
-      </c>
-      <c r="H8" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="I8" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="J8" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="K8" s="6" t="s">
-        <v>36</v>
-      </c>
+      <c r="M8" s="1"/>
       <c r="N8" s="1"/>
       <c r="O8" s="1"/>
-      <c r="P8" s="1"/>
     </row>
     <row r="9" ht="14.25">
-      <c r="A9" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="B9" s="6">
+      <c r="A9" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9" s="7">
         <v>8</v>
       </c>
-      <c r="C9" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="D9" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="E9" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="F9" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="G9" s="6">
-        <v>10</v>
-      </c>
-      <c r="H9" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="I9" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="J9" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="K9" s="6" t="s">
+      <c r="C9" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="D9" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="E9" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="F9" s="7" t="s">
         <v>36</v>
       </c>
+      <c r="G9" s="7">
+        <v>10</v>
+      </c>
+      <c r="H9" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="I9" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="J9" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="M9" s="1"/>
       <c r="N9" s="1"/>
       <c r="O9" s="1"/>
-      <c r="P9" s="1"/>
     </row>
     <row r="10" ht="14.25">
-      <c r="A10" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="B10" s="7">
+      <c r="A10" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="B10" s="9">
         <v>9</v>
       </c>
-      <c r="C10" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="D10" s="7" t="s">
+      <c r="C10" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="D10" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="E10" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="F10" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="E10" s="7" t="s">
+      <c r="G10" s="9"/>
+      <c r="H10" s="9"/>
+      <c r="I10" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="F10" s="8" t="s">
+      <c r="J10" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="G10" s="7"/>
-      <c r="H10" s="7"/>
-      <c r="I10" s="7"/>
-      <c r="J10" s="7"/>
-      <c r="K10" s="7" t="s">
-        <v>42</v>
-      </c>
+      <c r="M10" s="1"/>
       <c r="N10" s="1"/>
       <c r="O10" s="1"/>
-      <c r="P10" s="1"/>
     </row>
     <row r="11" ht="14.25">
       <c r="A11" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B11">
         <v>10</v>
       </c>
-      <c r="G11" s="9"/>
-      <c r="H11" s="9"/>
+      <c r="G11" s="11"/>
+      <c r="H11" s="1"/>
       <c r="I11" s="1"/>
-      <c r="J11" s="1"/>
+      <c r="M11" s="1"/>
       <c r="N11" s="1"/>
       <c r="O11" s="1"/>
-      <c r="P11" s="1"/>
     </row>
     <row r="12" ht="14.25">
       <c r="A12" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B12">
         <v>11</v>
       </c>
-      <c r="G12" s="9"/>
-      <c r="H12" s="9"/>
+      <c r="G12" s="11"/>
+      <c r="H12" s="1"/>
       <c r="I12" s="1"/>
-      <c r="J12" s="1"/>
+      <c r="M12" s="1"/>
       <c r="N12" s="1"/>
       <c r="O12" s="1"/>
-      <c r="P12" s="1"/>
     </row>
     <row r="13" ht="14.25">
       <c r="A13" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B13">
         <v>12</v>
       </c>
-      <c r="G13" s="9"/>
-      <c r="H13" s="9"/>
+      <c r="G13" s="11"/>
+      <c r="H13" s="1"/>
       <c r="I13" s="1"/>
-      <c r="J13" s="1"/>
+      <c r="M13" s="1"/>
       <c r="N13" s="1"/>
       <c r="O13" s="1"/>
-      <c r="P13" s="1"/>
     </row>
     <row r="14" ht="14.25">
-      <c r="A14" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="B14" s="10">
+      <c r="A14" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="B14" s="12">
         <v>13</v>
       </c>
-      <c r="C14" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="D14" s="10" t="s">
+      <c r="C14" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="D14" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="E14" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="F14" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="E14" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="F14" s="10" t="s">
+      <c r="G14" s="12">
+        <v>34</v>
+      </c>
+      <c r="H14" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="I14" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="J14" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="G14" s="10">
-        <v>34</v>
-      </c>
-      <c r="H14" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="I14" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="J14" s="10"/>
-      <c r="K14" s="10" t="s">
-        <v>45</v>
-      </c>
+      <c r="M14" s="1"/>
       <c r="N14" s="1"/>
       <c r="O14" s="1"/>
-      <c r="P14" s="1"/>
     </row>
     <row r="15" ht="14.25">
-      <c r="A15" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="B15" s="10">
+      <c r="A15" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="B15" s="12">
         <v>14</v>
       </c>
-      <c r="C15" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="D15" s="10" t="s">
-        <v>43</v>
-      </c>
-      <c r="E15" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="F15" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="G15" s="10">
+      <c r="C15" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="D15" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="E15" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="F15" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="G15" s="12">
         <v>116</v>
       </c>
-      <c r="H15" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="I15" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="J15" s="10"/>
-      <c r="K15" s="10" t="s">
-        <v>45</v>
-      </c>
+      <c r="H15" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="I15" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="J15" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="M15" s="1"/>
       <c r="N15" s="1"/>
       <c r="O15" s="1"/>
-      <c r="P15" s="1"/>
     </row>
     <row r="16" ht="14.25">
-      <c r="A16" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="B16" s="10">
+      <c r="A16" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="B16" s="12">
         <v>15</v>
       </c>
-      <c r="C16" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="D16" s="10" t="s">
-        <v>43</v>
-      </c>
-      <c r="E16" s="10" t="s">
+      <c r="C16" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="D16" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="E16" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="F16" s="12" t="s">
         <v>47</v>
       </c>
-      <c r="F16" s="10" t="s">
+      <c r="G16" s="12"/>
+      <c r="H16" s="12" t="s">
         <v>48</v>
       </c>
-      <c r="G16" s="10"/>
-      <c r="H16" s="10"/>
-      <c r="I16" s="10" t="s">
-        <v>49</v>
-      </c>
-      <c r="J16" s="10"/>
-      <c r="K16" s="10" t="s">
-        <v>45</v>
-      </c>
+      <c r="I16" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="J16" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="M16" s="1"/>
       <c r="N16" s="1"/>
       <c r="O16" s="1"/>
-      <c r="P16" s="1"/>
     </row>
     <row r="17" ht="14.25">
-      <c r="A17" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="B17" s="10">
+      <c r="A17" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="B17" s="12">
         <v>16</v>
       </c>
-      <c r="C17" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="D17" s="10" t="s">
-        <v>43</v>
-      </c>
-      <c r="E17" s="10" t="s">
+      <c r="C17" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="D17" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="E17" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="F17" s="12" t="s">
         <v>50</v>
       </c>
-      <c r="F17" s="10" t="s">
+      <c r="G17" s="12"/>
+      <c r="H17" s="12" t="s">
         <v>51</v>
       </c>
-      <c r="G17" s="10"/>
-      <c r="H17" s="10"/>
-      <c r="I17" s="10" t="s">
-        <v>52</v>
-      </c>
-      <c r="J17" s="10"/>
-      <c r="K17" s="10" t="s">
-        <v>45</v>
-      </c>
+      <c r="I17" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="J17" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="M17" s="1"/>
       <c r="N17" s="1"/>
       <c r="O17" s="1"/>
-      <c r="P17" s="1"/>
     </row>
     <row r="18" ht="14.25">
-      <c r="A18" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="B18" s="10">
+      <c r="A18" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="B18" s="12">
         <v>17</v>
       </c>
-      <c r="C18" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="D18" s="10" t="s">
-        <v>43</v>
-      </c>
-      <c r="E18" s="10" t="s">
+      <c r="C18" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="D18" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="E18" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="F18" s="12" t="s">
         <v>53</v>
       </c>
-      <c r="F18" s="10" t="s">
-        <v>54</v>
-      </c>
-      <c r="G18" s="10">
+      <c r="G18" s="12">
         <v>6</v>
       </c>
-      <c r="H18" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="I18" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="J18" s="10"/>
-      <c r="K18" s="10" t="s">
-        <v>45</v>
-      </c>
+      <c r="H18" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="I18" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="J18" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="M18" s="1"/>
       <c r="N18" s="1"/>
       <c r="O18" s="1"/>
-      <c r="P18" s="1"/>
     </row>
     <row r="19" ht="14.25">
       <c r="A19" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B19">
         <v>18</v>
       </c>
-      <c r="G19" s="9"/>
-      <c r="H19" s="9"/>
-      <c r="I19" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="J19" s="1"/>
+      <c r="G19" s="11"/>
+      <c r="H19" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="I19" s="1"/>
+      <c r="M19" s="1"/>
       <c r="N19" s="1"/>
       <c r="O19" s="1"/>
-      <c r="P19" s="1"/>
     </row>
     <row r="20" ht="14.25">
-      <c r="A20" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="B20" s="11">
+      <c r="A20" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="B20" s="13">
         <v>19</v>
       </c>
-      <c r="C20" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="D20" s="11" t="s">
+      <c r="C20" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="D20" s="13" t="s">
+        <v>55</v>
+      </c>
+      <c r="E20" s="13" t="s">
         <v>56</v>
       </c>
-      <c r="E20" s="11" t="s">
+      <c r="F20" s="13" t="s">
         <v>57</v>
       </c>
-      <c r="F20" s="11" t="s">
+      <c r="G20" s="13">
+        <v>15</v>
+      </c>
+      <c r="H20" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="I20" s="14" t="s">
         <v>58</v>
       </c>
-      <c r="G20" s="11">
-        <v>15</v>
-      </c>
-      <c r="H20" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="I20" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="J20" s="11" t="s">
+      <c r="J20" s="13" t="s">
         <v>59</v>
       </c>
-      <c r="K20" s="11" t="s">
-        <v>60</v>
-      </c>
+      <c r="M20" s="1"/>
       <c r="N20" s="1"/>
       <c r="O20" s="1"/>
-      <c r="P20" s="1"/>
     </row>
     <row r="21" ht="14.25">
-      <c r="A21" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="B21" s="11">
+      <c r="A21" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="B21" s="13">
         <v>20</v>
       </c>
-      <c r="C21" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="D21" s="11" t="s">
-        <v>56</v>
-      </c>
-      <c r="E21" s="11" t="s">
+      <c r="C21" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="D21" s="13" t="s">
+        <v>55</v>
+      </c>
+      <c r="E21" s="13" t="s">
+        <v>60</v>
+      </c>
+      <c r="F21" s="13" t="s">
         <v>61</v>
       </c>
-      <c r="F21" s="11" t="s">
-        <v>62</v>
-      </c>
-      <c r="G21" s="11"/>
-      <c r="H21" s="11"/>
-      <c r="I21" s="11" t="s">
-        <v>55</v>
-      </c>
-      <c r="J21" s="11"/>
-      <c r="K21" s="11" t="s">
-        <v>60</v>
-      </c>
+      <c r="G21" s="13"/>
+      <c r="H21" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="I21" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="J21" s="13" t="s">
+        <v>59</v>
+      </c>
+      <c r="M21" s="1"/>
       <c r="N21" s="1"/>
       <c r="O21" s="1"/>
-      <c r="P21" s="1"/>
     </row>
     <row r="22" ht="14.25">
-      <c r="A22" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="B22" s="11">
+      <c r="A22" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="B22" s="13">
         <v>21</v>
       </c>
-      <c r="C22" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="D22" s="11" t="s">
-        <v>56</v>
-      </c>
-      <c r="E22" s="11" t="s">
+      <c r="C22" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="D22" s="13" t="s">
+        <v>55</v>
+      </c>
+      <c r="E22" s="13" t="s">
+        <v>62</v>
+      </c>
+      <c r="F22" s="13" t="s">
         <v>63</v>
       </c>
-      <c r="F22" s="11" t="s">
+      <c r="G22" s="13">
+        <v>39</v>
+      </c>
+      <c r="H22" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="I22" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="J22" s="13" t="s">
+        <v>59</v>
+      </c>
+      <c r="N22" s="1"/>
+      <c r="O22" s="1"/>
+    </row>
+    <row r="23" ht="14.25">
+      <c r="A23" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="B23" s="13">
+        <v>22</v>
+      </c>
+      <c r="C23" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="D23" s="13" t="s">
+        <v>55</v>
+      </c>
+      <c r="E23" s="13" t="s">
         <v>64</v>
       </c>
-      <c r="G22" s="11">
-        <v>39</v>
-      </c>
-      <c r="H22" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="I22" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="J22" s="11"/>
-      <c r="K22" s="11" t="s">
-        <v>60</v>
-      </c>
-      <c r="O22" s="1"/>
-      <c r="P22" s="1"/>
-    </row>
-    <row r="23" ht="14.25">
-      <c r="A23" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="B23" s="11">
-        <v>22</v>
-      </c>
-      <c r="C23" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="D23" s="11" t="s">
-        <v>56</v>
-      </c>
-      <c r="E23" s="11" t="s">
+      <c r="F23" s="13" t="s">
         <v>65</v>
       </c>
-      <c r="F23" s="11" t="s">
+      <c r="G23" s="13">
+        <v>23</v>
+      </c>
+      <c r="H23" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="I23" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="J23" s="13" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="24" ht="14.25">
+      <c r="A24" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="B24" s="13">
+        <v>23</v>
+      </c>
+      <c r="C24" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="D24" s="13" t="s">
+        <v>55</v>
+      </c>
+      <c r="E24" s="13" t="s">
         <v>66</v>
       </c>
-      <c r="G23" s="11">
-        <v>23</v>
-      </c>
-      <c r="H23" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="I23" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="J23" s="11"/>
-      <c r="K23" s="11" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="24" ht="14.25">
-      <c r="A24" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="B24" s="11">
-        <v>23</v>
-      </c>
-      <c r="C24" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="D24" s="11" t="s">
-        <v>56</v>
-      </c>
-      <c r="E24" s="11" t="s">
+      <c r="F24" s="13" t="s">
         <v>67</v>
       </c>
-      <c r="F24" s="11" t="s">
+      <c r="G24" s="13">
+        <v>43</v>
+      </c>
+      <c r="H24" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="I24" s="14" t="s">
+        <v>58</v>
+      </c>
+      <c r="J24" s="13" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="25" ht="14.25">
+      <c r="A25" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="B25" s="13">
+        <v>24</v>
+      </c>
+      <c r="C25" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="D25" s="13" t="s">
+        <v>55</v>
+      </c>
+      <c r="E25" s="13" t="s">
         <v>68</v>
       </c>
-      <c r="G24" s="11">
-        <v>43</v>
-      </c>
-      <c r="H24" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="I24" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="J24" s="11" t="s">
+      <c r="F25" s="13" t="s">
+        <v>69</v>
+      </c>
+      <c r="G25" s="13">
+        <v>28</v>
+      </c>
+      <c r="H25" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="I25" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="J25" s="13" t="s">
         <v>59</v>
       </c>
-      <c r="K24" s="11" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="25" ht="14.25">
-      <c r="A25" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="B25" s="11">
-        <v>24</v>
-      </c>
-      <c r="C25" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="D25" s="11" t="s">
-        <v>56</v>
-      </c>
-      <c r="E25" s="11" t="s">
-        <v>69</v>
-      </c>
-      <c r="F25" s="11" t="s">
+    </row>
+    <row r="26" ht="14.25">
+      <c r="A26" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="B26" s="13">
+        <v>25</v>
+      </c>
+      <c r="C26" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="D26" s="13" t="s">
+        <v>55</v>
+      </c>
+      <c r="E26" s="13" t="s">
         <v>70</v>
       </c>
-      <c r="G25" s="11">
+      <c r="F26" s="13" t="s">
+        <v>71</v>
+      </c>
+      <c r="G26" s="13">
+        <v>54</v>
+      </c>
+      <c r="H26" s="13" t="s">
+        <v>72</v>
+      </c>
+      <c r="I26" s="14" t="s">
+        <v>58</v>
+      </c>
+      <c r="J26" s="13" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="27" ht="14.25">
+      <c r="A27" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="B27" s="13">
+        <v>26</v>
+      </c>
+      <c r="C27" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="D27" s="13" t="s">
+        <v>55</v>
+      </c>
+      <c r="E27" s="13" t="s">
+        <v>73</v>
+      </c>
+      <c r="F27" s="13" t="s">
+        <v>74</v>
+      </c>
+      <c r="G27" s="13">
+        <v>53</v>
+      </c>
+      <c r="H27" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="I27" s="14" t="s">
+        <v>58</v>
+      </c>
+      <c r="J27" s="13" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="28" ht="14.25">
+      <c r="A28" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="B28" s="13">
+        <v>27</v>
+      </c>
+      <c r="C28" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="D28" s="13" t="s">
+        <v>55</v>
+      </c>
+      <c r="E28" s="13" t="s">
+        <v>75</v>
+      </c>
+      <c r="F28" s="13" t="s">
+        <v>76</v>
+      </c>
+      <c r="G28" s="13">
+        <v>54</v>
+      </c>
+      <c r="H28" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="I28" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="J28" s="13" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="29" ht="14.25">
+      <c r="A29" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="B29" s="13">
         <v>28</v>
       </c>
-      <c r="H25" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="I25" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="J25" s="11"/>
-      <c r="K25" s="11" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="26" ht="14.25">
-      <c r="A26" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="B26" s="11">
-        <v>25</v>
-      </c>
-      <c r="C26" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="D26" s="11" t="s">
-        <v>56</v>
-      </c>
-      <c r="E26" s="11" t="s">
-        <v>71</v>
-      </c>
-      <c r="F26" s="11" t="s">
-        <v>72</v>
-      </c>
-      <c r="G26" s="11">
-        <v>54</v>
-      </c>
-      <c r="H26" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="I26" s="11" t="s">
-        <v>73</v>
-      </c>
-      <c r="J26" s="11" t="s">
+      <c r="C29" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="D29" s="13" t="s">
+        <v>55</v>
+      </c>
+      <c r="E29" s="13" t="s">
+        <v>77</v>
+      </c>
+      <c r="F29" s="13" t="s">
+        <v>78</v>
+      </c>
+      <c r="G29" s="13"/>
+      <c r="H29" s="13" t="s">
+        <v>48</v>
+      </c>
+      <c r="I29" s="14" t="s">
+        <v>58</v>
+      </c>
+      <c r="J29" s="13" t="s">
         <v>59</v>
-      </c>
-      <c r="K26" s="11" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="27" ht="14.25">
-      <c r="A27" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="B27" s="11">
-        <v>26</v>
-      </c>
-      <c r="C27" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="D27" s="11" t="s">
-        <v>56</v>
-      </c>
-      <c r="E27" s="11" t="s">
-        <v>74</v>
-      </c>
-      <c r="F27" s="11" t="s">
-        <v>75</v>
-      </c>
-      <c r="G27" s="11">
-        <v>53</v>
-      </c>
-      <c r="H27" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="I27" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="J27" s="11" t="s">
-        <v>59</v>
-      </c>
-      <c r="K27" s="11" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="28" ht="14.25">
-      <c r="A28" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="B28" s="11">
-        <v>27</v>
-      </c>
-      <c r="C28" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="D28" s="11" t="s">
-        <v>56</v>
-      </c>
-      <c r="E28" s="11" t="s">
-        <v>76</v>
-      </c>
-      <c r="F28" s="11" t="s">
-        <v>77</v>
-      </c>
-      <c r="G28" s="11">
-        <v>54</v>
-      </c>
-      <c r="H28" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="I28" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="J28" s="11"/>
-      <c r="K28" s="11" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="29" ht="14.25">
-      <c r="A29" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="B29" s="11">
-        <v>28</v>
-      </c>
-      <c r="C29" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="D29" s="11" t="s">
-        <v>56</v>
-      </c>
-      <c r="E29" s="11" t="s">
-        <v>78</v>
-      </c>
-      <c r="F29" s="11" t="s">
-        <v>79</v>
-      </c>
-      <c r="G29" s="11"/>
-      <c r="H29" s="11"/>
-      <c r="I29" s="11" t="s">
-        <v>49</v>
-      </c>
-      <c r="J29" s="11" t="s">
-        <v>59</v>
-      </c>
-      <c r="K29" s="11" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="30" ht="14.25">
       <c r="A30" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B30">
         <v>29</v>
       </c>
       <c r="C30" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E30" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F30" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="G30" s="1">
         <v>65</v>
       </c>
       <c r="H30" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="I30" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="J30" s="1"/>
+        <v>48</v>
+      </c>
+      <c r="I30" s="1"/>
     </row>
     <row r="31" ht="14.25">
       <c r="A31" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B31">
         <v>30</v>
       </c>
       <c r="C31" t="s">
-        <v>12</v>
-      </c>
-      <c r="F31" s="12" t="s">
-        <v>81</v>
-      </c>
-      <c r="G31" s="12">
+        <v>11</v>
+      </c>
+      <c r="F31" s="15" t="s">
+        <v>80</v>
+      </c>
+      <c r="G31" s="15">
         <v>59</v>
       </c>
-      <c r="H31" s="12" t="s">
-        <v>16</v>
-      </c>
+      <c r="K31"/>
+      <c r="L31"/>
     </row>
     <row r="32" ht="14.25">
       <c r="A32" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B32">
         <v>31</v>
       </c>
       <c r="C32" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D32" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="F32" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="F32" s="1" t="s">
+      <c r="I32" t="s">
         <v>83</v>
       </c>
       <c r="J32" t="s">
         <v>84</v>
       </c>
+      <c r="K32" s="1"/>
+      <c r="L32" s="1"/>
     </row>
     <row r="33" ht="14.25">
       <c r="A33" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B33">
         <v>32</v>
       </c>
-      <c r="C33" s="9" t="s">
-        <v>12</v>
+      <c r="C33" s="11" t="s">
+        <v>11</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F33" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="J33" s="9" t="s">
+      <c r="I33" s="11" t="s">
+        <v>83</v>
+      </c>
+      <c r="J33" t="s">
         <v>84</v>
       </c>
+      <c r="K33" s="1"/>
+      <c r="L33" s="1"/>
     </row>
     <row r="34" ht="14.25">
       <c r="A34" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B34">
         <v>33</v>
       </c>
-      <c r="C34" s="9" t="s">
-        <v>12</v>
+      <c r="C34" s="11" t="s">
+        <v>11</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F34" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="J34" s="9" t="s">
+      <c r="I34" s="11" t="s">
+        <v>83</v>
+      </c>
+      <c r="J34" t="s">
         <v>84</v>
       </c>
+      <c r="K34" s="1"/>
+      <c r="L34" s="1"/>
     </row>
     <row r="35" ht="14.25">
       <c r="A35" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B35">
         <v>34</v>
       </c>
-      <c r="C35" s="9" t="s">
-        <v>12</v>
+      <c r="C35" s="11" t="s">
+        <v>11</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F35" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="J35" s="9" t="s">
+      <c r="I35" s="11" t="s">
+        <v>83</v>
+      </c>
+      <c r="J35" t="s">
         <v>84</v>
       </c>
+      <c r="K35" s="1"/>
+      <c r="L35" s="1"/>
     </row>
     <row r="36" ht="14.25">
       <c r="A36" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B36">
         <v>35</v>
       </c>
-      <c r="C36" s="9" t="s">
-        <v>12</v>
+      <c r="C36" s="11" t="s">
+        <v>11</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F36" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="J36" s="9" t="s">
+      <c r="I36" s="11" t="s">
+        <v>83</v>
+      </c>
+      <c r="J36" t="s">
         <v>84</v>
       </c>
+      <c r="K36" s="1"/>
+      <c r="L36" s="1"/>
     </row>
     <row r="37" ht="14.25">
       <c r="A37" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B37">
         <v>36</v>
       </c>
-      <c r="C37" s="9" t="s">
-        <v>12</v>
+      <c r="C37" s="11" t="s">
+        <v>11</v>
       </c>
       <c r="D37" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="F37" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="F37" s="1" t="s">
+      <c r="I37" s="11" t="s">
         <v>83</v>
       </c>
-      <c r="J37" s="9" t="s">
+      <c r="J37" t="s">
         <v>84</v>
       </c>
+      <c r="K37" s="1"/>
+      <c r="L37" s="1"/>
     </row>
     <row r="38" ht="14.25">
       <c r="A38" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B38">
         <v>37</v>
       </c>
-      <c r="C38" s="9" t="s">
-        <v>12</v>
+      <c r="C38" s="11" t="s">
+        <v>11</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F38" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="J38" s="9" t="s">
+      <c r="I38" s="11" t="s">
+        <v>83</v>
+      </c>
+      <c r="J38" t="s">
         <v>84</v>
       </c>
+      <c r="K38" s="1"/>
+      <c r="L38" s="1"/>
     </row>
     <row r="39" ht="14.25">
       <c r="A39" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B39">
         <v>38</v>
       </c>
-      <c r="C39" s="9" t="s">
-        <v>12</v>
+      <c r="C39" s="11" t="s">
+        <v>11</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F39" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="J39" s="9" t="s">
+      <c r="I39" s="11" t="s">
+        <v>83</v>
+      </c>
+      <c r="J39" t="s">
         <v>84</v>
       </c>
+      <c r="K39" s="1"/>
+      <c r="L39" s="1"/>
     </row>
     <row r="40" ht="14.25">
       <c r="A40" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B40">
         <v>39</v>
       </c>
-      <c r="C40" s="9" t="s">
-        <v>12</v>
+      <c r="C40" s="11" t="s">
+        <v>11</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F40" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="J40" s="9" t="s">
+      <c r="I40" s="11" t="s">
+        <v>83</v>
+      </c>
+      <c r="J40" t="s">
         <v>84</v>
       </c>
+      <c r="K40" s="1"/>
+      <c r="L40" s="1"/>
     </row>
     <row r="41" ht="14.25">
       <c r="A41" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B41">
         <v>40</v>
       </c>
-      <c r="C41" s="9" t="s">
-        <v>12</v>
+      <c r="C41" s="11" t="s">
+        <v>11</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F41" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="J41" s="9" t="s">
+      <c r="I41" s="11" t="s">
+        <v>83</v>
+      </c>
+      <c r="J41" t="s">
         <v>84</v>
       </c>
+      <c r="K41" s="1"/>
+      <c r="L41" s="1"/>
     </row>
     <row r="42" ht="14.25">
       <c r="A42" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B42">
         <v>41</v>
       </c>
-      <c r="C42" s="9" t="s">
-        <v>12</v>
+      <c r="C42" s="11" t="s">
+        <v>11</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F42" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="J42" s="9" t="s">
+      <c r="I42" s="11" t="s">
+        <v>83</v>
+      </c>
+      <c r="J42" t="s">
         <v>84</v>
       </c>
+      <c r="K42" s="1"/>
+      <c r="L42" s="1"/>
     </row>
     <row r="43" ht="14.25">
       <c r="A43" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B43">
         <v>42</v>
       </c>
-      <c r="C43" s="9" t="s">
-        <v>12</v>
+      <c r="C43" s="11" t="s">
+        <v>11</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F43" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="J43" s="9" t="s">
+      <c r="I43" s="11" t="s">
+        <v>83</v>
+      </c>
+      <c r="J43" t="s">
         <v>84</v>
       </c>
+      <c r="K43" s="1"/>
+      <c r="L43" s="1"/>
     </row>
     <row r="44" ht="14.25">
       <c r="A44" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B44">
         <v>43</v>
       </c>
-      <c r="C44" s="9" t="s">
-        <v>12</v>
+      <c r="C44" s="11" t="s">
+        <v>11</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F44" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="J44" s="9" t="s">
+      <c r="I44" s="11" t="s">
+        <v>83</v>
+      </c>
+      <c r="J44" t="s">
         <v>84</v>
       </c>
+      <c r="K44" s="1"/>
+      <c r="L44" s="1"/>
     </row>
     <row r="45" ht="14.25">
       <c r="A45" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B45">
         <v>44</v>
       </c>
-      <c r="C45" s="9" t="s">
-        <v>12</v>
+      <c r="C45" s="11" t="s">
+        <v>11</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F45" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="J45" s="9" t="s">
+      <c r="I45" s="11" t="s">
+        <v>83</v>
+      </c>
+      <c r="J45" t="s">
         <v>84</v>
       </c>
+      <c r="K45" s="1"/>
+      <c r="L45" s="1"/>
     </row>
     <row r="46" ht="14.25">
       <c r="A46" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B46">
         <v>45</v>
       </c>
-      <c r="C46" s="9" t="s">
-        <v>12</v>
+      <c r="C46" s="11" t="s">
+        <v>11</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F46" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="J46" s="9" t="s">
+      <c r="I46" s="11" t="s">
+        <v>83</v>
+      </c>
+      <c r="J46" t="s">
         <v>84</v>
       </c>
+      <c r="K46" s="1"/>
+      <c r="L46" s="1"/>
     </row>
     <row r="47" ht="14.25">
       <c r="A47" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B47">
         <v>46</v>
       </c>
-      <c r="C47" s="9" t="s">
-        <v>12</v>
+      <c r="C47" s="11" t="s">
+        <v>11</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F47" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="J47" s="9" t="s">
+      <c r="I47" s="11" t="s">
+        <v>83</v>
+      </c>
+      <c r="J47" t="s">
         <v>84</v>
       </c>
+      <c r="K47" s="1"/>
+      <c r="L47" s="1"/>
     </row>
     <row r="48" ht="14.25">
       <c r="A48" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B48">
         <v>47</v>
       </c>
-      <c r="C48" s="9" t="s">
-        <v>12</v>
+      <c r="C48" s="11" t="s">
+        <v>11</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F48" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="J48" s="9" t="s">
+      <c r="I48" s="11" t="s">
+        <v>83</v>
+      </c>
+      <c r="J48" t="s">
         <v>84</v>
       </c>
+      <c r="K48" s="1"/>
+      <c r="L48" s="1"/>
     </row>
     <row r="49" ht="14.25">
       <c r="A49" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B49">
         <v>48</v>
       </c>
-      <c r="C49" s="9" t="s">
-        <v>12</v>
+      <c r="C49" s="11" t="s">
+        <v>11</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F49" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="J49" s="9" t="s">
+      <c r="I49" s="11" t="s">
+        <v>83</v>
+      </c>
+      <c r="J49" t="s">
         <v>84</v>
       </c>
+      <c r="K49" s="1"/>
+      <c r="L49" s="1"/>
     </row>
     <row r="50" ht="14.25">
       <c r="A50" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B50">
         <v>49</v>
       </c>
-      <c r="C50" s="9" t="s">
-        <v>12</v>
+      <c r="C50" s="11" t="s">
+        <v>11</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F50" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="J50" s="9" t="s">
+      <c r="I50" s="11" t="s">
+        <v>83</v>
+      </c>
+      <c r="J50" t="s">
         <v>84</v>
       </c>
+      <c r="K50" s="1"/>
+      <c r="L50" s="1"/>
     </row>
     <row r="51" ht="14.25">
       <c r="A51" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B51">
         <v>50</v>
       </c>
-      <c r="C51" s="9" t="s">
-        <v>12</v>
+      <c r="C51" s="11" t="s">
+        <v>11</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F51" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="J51" s="9" t="s">
+      <c r="I51" s="11" t="s">
+        <v>83</v>
+      </c>
+      <c r="J51" t="s">
         <v>84</v>
       </c>
+      <c r="K51" s="1"/>
+      <c r="L51" s="1"/>
     </row>
     <row r="52" ht="14.25">
       <c r="A52" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B52">
         <v>51</v>
       </c>
-      <c r="C52" s="9" t="s">
-        <v>12</v>
+      <c r="C52" s="11" t="s">
+        <v>11</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F52" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="J52" s="9" t="s">
+      <c r="I52" s="11" t="s">
+        <v>83</v>
+      </c>
+      <c r="J52" t="s">
         <v>84</v>
       </c>
+      <c r="K52" s="1"/>
+      <c r="L52" s="1"/>
     </row>
     <row r="53" ht="14.25">
       <c r="A53" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B53">
         <v>52</v>
       </c>
-      <c r="C53" s="9" t="s">
-        <v>12</v>
+      <c r="C53" s="11" t="s">
+        <v>11</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F53" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="J53" s="9" t="s">
+      <c r="I53" s="11" t="s">
+        <v>83</v>
+      </c>
+      <c r="J53" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="54" ht="14.25"/>
+      <c r="K53" s="1"/>
+      <c r="L53" s="1"/>
+    </row>
+    <row r="54" ht="14.25">
+      <c r="K54"/>
+      <c r="L54" s="1"/>
+    </row>
+    <row r="55" ht="14.25">
+      <c r="K55"/>
+      <c r="L55"/>
+    </row>
   </sheetData>
   <printOptions headings="0" gridLines="0"/>
   <pageMargins left="0.70078740157480324" right="0.70078740157480324" top="0.75196850393700787" bottom="0.75196850393700787" header="0.29999999999999999" footer="0.29999999999999999"/>
@@ -2551,7 +2621,7 @@
         <v>96</v>
       </c>
       <c r="B2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C2" t="s">
         <v>97</v>
@@ -2565,7 +2635,7 @@
         <v>99</v>
       </c>
       <c r="B3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C3" t="s">
         <v>100</v>
@@ -2579,7 +2649,7 @@
         <v>102</v>
       </c>
       <c r="B4" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C4" t="s">
         <v>103</v>
@@ -2593,7 +2663,7 @@
         <v>104</v>
       </c>
       <c r="B5" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C5" t="s">
         <v>100</v>
@@ -2607,7 +2677,7 @@
         <v>105</v>
       </c>
       <c r="B6" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C6" t="s">
         <v>106</v>
@@ -2621,7 +2691,7 @@
         <v>107</v>
       </c>
       <c r="B7" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C7" t="s">
         <v>108</v>
@@ -2635,7 +2705,7 @@
         <v>109</v>
       </c>
       <c r="B8" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C8" t="s">
         <v>106</v>
@@ -2649,7 +2719,7 @@
         <v>110</v>
       </c>
       <c r="B9" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C9" t="s">
         <v>111</v>
@@ -2660,7 +2730,7 @@
     </row>
     <row r="10">
       <c r="B10" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C10" t="s">
         <v>112</v>
@@ -2671,7 +2741,7 @@
     </row>
     <row r="11">
       <c r="B11" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C11" t="s">
         <v>106</v>
@@ -2682,7 +2752,7 @@
     </row>
     <row r="12">
       <c r="B12" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C12" t="s">
         <v>108</v>
@@ -2696,7 +2766,7 @@
         <v>113</v>
       </c>
       <c r="B13" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C13" t="s">
         <v>106</v>
@@ -2707,7 +2777,7 @@
     </row>
     <row r="14">
       <c r="B14" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C14" t="s">
         <v>97</v>
@@ -2718,7 +2788,7 @@
     </row>
     <row r="15">
       <c r="B15" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C15" t="s">
         <v>106</v>
@@ -2732,7 +2802,7 @@
         <v>114</v>
       </c>
       <c r="B16" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C16" t="s">
         <v>106</v>
@@ -2743,7 +2813,7 @@
     </row>
     <row r="17">
       <c r="B17" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C17" t="s">
         <v>106</v>
@@ -2754,7 +2824,7 @@
     </row>
     <row r="18">
       <c r="B18" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D18" t="s">
         <v>101</v>
@@ -2765,7 +2835,7 @@
         <v>115</v>
       </c>
       <c r="B19" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C19">
         <v>35</v>
@@ -2779,7 +2849,7 @@
         <v>116</v>
       </c>
       <c r="B20" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C20" t="s">
         <v>112</v>
@@ -2790,7 +2860,7 @@
     </row>
     <row r="21">
       <c r="B21" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C21" t="s">
         <v>106</v>
@@ -2801,7 +2871,7 @@
     </row>
     <row r="22">
       <c r="B22" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C22" t="s">
         <v>111</v>
@@ -2813,7 +2883,7 @@
     <row r="23" ht="14.25">
       <c r="A23" s="1"/>
       <c r="B23" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="24" ht="14.25">

</xml_diff>

<commit_message>
Changes to BCB dataset script. Improved sample overview, merge between both old versions. Updated conda env on server. Changed standard workflow to remote jupyter notebooks.
</commit_message>
<xml_diff>
--- a/docs/overview.xlsx
+++ b/docs/overview.xlsx
@@ -4,7 +4,7 @@
   <workbookPr date1904="0"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="15" windowWidth="20955" windowHeight="9720" activeTab="2"/>
+    <workbookView xWindow="360" yWindow="15" windowWidth="20955" windowHeight="9720" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="libraries" sheetId="1" state="visible" r:id="rId1"/>
@@ -501,6 +501,12 @@
     <t>outcome</t>
   </si>
   <si>
+    <t>onset</t>
+  </si>
+  <si>
+    <t>vaccine_status</t>
+  </si>
+  <si>
     <t>SCoV2_variant</t>
   </si>
   <si>
@@ -663,9 +669,6 @@
     <t>C19-CB-0914</t>
   </si>
   <si>
-    <t>unknown</t>
-  </si>
-  <si>
     <t>BR3</t>
   </si>
   <si>
@@ -673,9 +676,6 @@
   </si>
   <si>
     <t>death</t>
-  </si>
-  <si>
-    <t>NA</t>
   </si>
   <si>
     <t>BR4</t>
@@ -1158,7 +1158,7 @@
       <sz val="11.000000"/>
     </font>
   </fonts>
-  <fills count="12">
+  <fills count="13">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1225,6 +1225,9 @@
         <bgColor rgb="FFFFF2CC"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="none"/>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -1254,7 +1257,7 @@
       <protection hidden="0" locked="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="39">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyProtection="0">
       <protection hidden="0" locked="1"/>
     </xf>
@@ -1293,28 +1296,65 @@
       <alignment wrapText="1"/>
       <protection hidden="0" locked="1"/>
     </xf>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyProtection="0">
+      <protection hidden="0" locked="1"/>
+    </xf>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyProtection="0">
+      <protection hidden="0" locked="1"/>
+    </xf>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="14" xfId="0" applyNumberFormat="1" applyProtection="0">
       <protection hidden="0" locked="1"/>
     </xf>
-    <xf fontId="3" fillId="3" borderId="0" numFmtId="0" xfId="7" applyFont="1" applyFill="1" applyProtection="0">
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="14" xfId="0" applyNumberFormat="1" applyProtection="0">
       <protection hidden="0" locked="1"/>
     </xf>
-    <xf fontId="3" fillId="3" borderId="0" numFmtId="14" xfId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyProtection="0">
+    <xf fontId="0" fillId="12" borderId="0" numFmtId="0" xfId="0" applyFill="1" applyProtection="0">
       <protection hidden="0" locked="1"/>
     </xf>
-    <xf fontId="4" fillId="4" borderId="0" numFmtId="0" xfId="8" applyFont="1" applyFill="1" applyProtection="0">
+    <xf fontId="0" fillId="12" borderId="0" numFmtId="0" xfId="0" applyFill="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left"/>
       <protection hidden="0" locked="1"/>
     </xf>
-    <xf fontId="4" fillId="4" borderId="0" numFmtId="14" xfId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyProtection="0">
-      <protection hidden="0" locked="1"/>
-    </xf>
-    <xf fontId="2" fillId="2" borderId="0" numFmtId="0" xfId="6" applyFont="1" applyFill="1" applyProtection="0">
-      <protection hidden="0" locked="1"/>
-    </xf>
-    <xf fontId="2" fillId="2" borderId="0" numFmtId="14" xfId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyProtection="0">
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyProtection="0">
       <protection hidden="0" locked="1"/>
     </xf>
     <xf fontId="7" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyProtection="0">
+      <protection hidden="0" locked="1"/>
+    </xf>
+    <xf fontId="7" fillId="0" borderId="0" numFmtId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyProtection="0">
+      <protection hidden="0" locked="1"/>
+    </xf>
+    <xf fontId="0" fillId="12" borderId="0" numFmtId="0" xfId="0" applyFill="1" applyProtection="0">
+      <protection hidden="0" locked="1"/>
+    </xf>
+    <xf fontId="7" fillId="12" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyProtection="0">
+      <protection hidden="0" locked="1"/>
+    </xf>
+    <xf fontId="7" fillId="12" borderId="0" numFmtId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyProtection="0">
+      <protection hidden="0" locked="1"/>
+    </xf>
+    <xf fontId="7" fillId="12" borderId="0" numFmtId="0" xfId="7" applyFont="1" applyFill="1" applyProtection="0">
+      <protection hidden="0" locked="1"/>
+    </xf>
+    <xf fontId="7" fillId="12" borderId="0" numFmtId="14" xfId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyProtection="0">
+      <protection hidden="0" locked="1"/>
+    </xf>
+    <xf fontId="7" fillId="12" borderId="0" numFmtId="14" xfId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyProtection="0">
+      <protection hidden="0" locked="1"/>
+    </xf>
+    <xf fontId="7" fillId="12" borderId="0" numFmtId="0" xfId="8" applyFont="1" applyFill="1" applyProtection="0">
+      <protection hidden="0" locked="1"/>
+    </xf>
+    <xf fontId="7" fillId="12" borderId="0" numFmtId="14" xfId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyProtection="0">
+      <protection hidden="0" locked="1"/>
+    </xf>
+    <xf fontId="7" fillId="12" borderId="0" numFmtId="14" xfId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyProtection="0">
+      <protection hidden="0" locked="1"/>
+    </xf>
+    <xf fontId="7" fillId="12" borderId="0" numFmtId="0" xfId="6" applyFont="1" applyFill="1" applyProtection="0">
+      <protection hidden="0" locked="1"/>
+    </xf>
+    <xf fontId="7" fillId="12" borderId="0" numFmtId="14" xfId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyProtection="0">
       <protection hidden="0" locked="1"/>
     </xf>
     <xf fontId="0" fillId="5" borderId="0" numFmtId="0" xfId="0" applyFill="1" applyAlignment="1" applyProtection="0">
@@ -3184,7 +3224,8 @@
     <pageSetUpPr autoPageBreaks="1" fitToPage="0"/>
   </sheetPr>
   <sheetViews>
-    <sheetView showGridLines="1" showRowColHeaders="1" showZeros="1" zoomScale="100" workbookViewId="0">
+    <sheetView showGridLines="1" showRowColHeaders="1" showZeros="1" topLeftCell="A1" zoomScale="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -3192,16 +3233,18 @@
   <cols>
     <col customWidth="1" min="2" max="3" style="0" width="12.880000000000001"/>
     <col bestFit="1" min="6" max="6" width="8.8515625"/>
-    <col bestFit="1" customWidth="1" min="7" max="7" style="0" width="13.140625"/>
-    <col customWidth="1" min="8" max="8" style="0" width="13.35"/>
-    <col customWidth="1" min="9" max="9" style="0" width="17.079999999999998"/>
-    <col customWidth="1" min="10" max="10" style="0" width="13.43"/>
-    <col customWidth="1" min="11" max="11" style="0" width="5.7300000000000004"/>
-    <col bestFit="1" customWidth="1" min="12" max="12" style="0" width="14.57421875"/>
-    <col customWidth="1" min="13" max="13" style="0" width="14.84"/>
-    <col customWidth="1" min="14" max="14" style="0" width="11.050000000000001"/>
-    <col customWidth="1" min="15" max="15" style="0" width="10.92"/>
-    <col customWidth="1" min="16" max="16" style="0" width="13.43"/>
+    <col bestFit="1" min="7" max="7" width="10.421875"/>
+    <col bestFit="1" min="8" max="8" width="13.28125"/>
+    <col bestFit="1" customWidth="1" min="9" max="9" style="0" width="13.140625"/>
+    <col customWidth="1" min="10" max="10" style="0" width="13.35"/>
+    <col customWidth="1" min="11" max="11" style="0" width="17.079999999999998"/>
+    <col customWidth="1" min="12" max="12" style="0" width="13.43"/>
+    <col customWidth="1" min="13" max="13" style="0" width="5.7300000000000004"/>
+    <col bestFit="1" customWidth="1" min="14" max="14" style="0" width="14.57421875"/>
+    <col customWidth="1" min="15" max="15" style="0" width="14.84"/>
+    <col customWidth="1" min="16" max="16" style="0" width="11.050000000000001"/>
+    <col customWidth="1" min="17" max="17" style="0" width="10.92"/>
+    <col customWidth="1" min="18" max="18" style="0" width="13.43"/>
   </cols>
   <sheetData>
     <row r="1" ht="14.25">
@@ -3223,55 +3266,66 @@
       <c r="F1" t="s">
         <v>159</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="12" t="s">
         <v>160</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="12" t="s">
         <v>161</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" t="s">
         <v>162</v>
       </c>
       <c r="J1" s="1" t="s">
         <v>163</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="K1" s="13" t="s">
         <v>164</v>
       </c>
-      <c r="L1" s="12" t="s">
+      <c r="L1" s="13" t="s">
         <v>165</v>
       </c>
-      <c r="M1" s="12" t="s">
+      <c r="M1" s="1" t="s">
         <v>166</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="N1" s="14" t="s">
         <v>167</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="O1" s="14" t="s">
         <v>168</v>
       </c>
       <c r="P1" s="1" t="s">
         <v>169</v>
       </c>
+      <c r="Q1" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>171</v>
+      </c>
     </row>
     <row r="2" ht="14.25">
+      <c r="A2" s="13"/>
       <c r="B2" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>19</v>
       </c>
       <c r="E2" t="s">
-        <v>171</v>
-      </c>
-      <c r="H2" s="12"/>
+        <v>173</v>
+      </c>
+      <c r="G2" s="15">
+        <v>43913</v>
+      </c>
+      <c r="H2" s="16"/>
+      <c r="J2" s="14"/>
     </row>
     <row r="3" ht="14.25">
       <c r="A3" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="B3" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>19</v>
@@ -3280,16 +3334,20 @@
         <v>72</v>
       </c>
       <c r="E3" t="s">
-        <v>174</v>
-      </c>
-      <c r="H3" s="12"/>
+        <v>176</v>
+      </c>
+      <c r="G3" s="15">
+        <v>43916</v>
+      </c>
+      <c r="H3" s="16"/>
+      <c r="J3" s="14"/>
     </row>
     <row r="4" ht="14.25">
       <c r="A4" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="B4" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>19</v>
@@ -3298,16 +3356,20 @@
         <v>56</v>
       </c>
       <c r="E4" t="s">
-        <v>171</v>
-      </c>
-      <c r="H4" s="12"/>
+        <v>173</v>
+      </c>
+      <c r="G4" s="15">
+        <v>43929</v>
+      </c>
+      <c r="H4" s="16"/>
+      <c r="J4" s="14"/>
     </row>
     <row r="5" ht="14.25">
       <c r="A5" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="B5" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>19</v>
@@ -3316,16 +3378,20 @@
         <v>72</v>
       </c>
       <c r="E5" t="s">
-        <v>174</v>
-      </c>
-      <c r="H5" s="12"/>
+        <v>176</v>
+      </c>
+      <c r="G5" s="15">
+        <v>43923</v>
+      </c>
+      <c r="H5" s="16"/>
+      <c r="J5" s="14"/>
     </row>
     <row r="6" ht="14.25">
       <c r="A6" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="B6" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>19</v>
@@ -3334,16 +3400,20 @@
         <v>63</v>
       </c>
       <c r="E6" t="s">
-        <v>174</v>
-      </c>
-      <c r="H6" s="12"/>
+        <v>176</v>
+      </c>
+      <c r="G6" s="15">
+        <v>43913</v>
+      </c>
+      <c r="H6" s="16"/>
+      <c r="J6" s="14"/>
     </row>
     <row r="7" ht="14.25">
       <c r="A7" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="B7" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>19</v>
@@ -3352,16 +3422,20 @@
         <v>22</v>
       </c>
       <c r="E7" t="s">
-        <v>174</v>
-      </c>
-      <c r="H7" s="12"/>
+        <v>176</v>
+      </c>
+      <c r="G7" s="15">
+        <v>43934</v>
+      </c>
+      <c r="H7" s="16"/>
+      <c r="J7" s="14"/>
     </row>
     <row r="8" ht="14.25">
       <c r="A8" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="B8" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>19</v>
@@ -3370,16 +3444,20 @@
         <v>62</v>
       </c>
       <c r="E8" t="s">
-        <v>171</v>
-      </c>
-      <c r="H8" s="12"/>
+        <v>173</v>
+      </c>
+      <c r="G8" s="15">
+        <v>43925</v>
+      </c>
+      <c r="H8" s="16"/>
+      <c r="J8" s="14"/>
     </row>
     <row r="9" ht="14.25">
       <c r="A9" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="B9" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>19</v>
@@ -3388,14 +3466,18 @@
         <v>75</v>
       </c>
       <c r="E9" t="s">
-        <v>174</v>
-      </c>
-      <c r="H9" s="12"/>
+        <v>176</v>
+      </c>
+      <c r="G9" s="15">
+        <v>43941</v>
+      </c>
+      <c r="H9" s="16"/>
+      <c r="J9" s="14"/>
     </row>
     <row r="10" ht="14.25">
-      <c r="A10" s="1"/>
+      <c r="A10" s="13"/>
       <c r="B10" s="1" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>63</v>
@@ -3404,13 +3486,18 @@
         <v>43</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>171</v>
-      </c>
-      <c r="H10" s="12"/>
+        <v>173</v>
+      </c>
+      <c r="G10" s="15">
+        <v>43979</v>
+      </c>
+      <c r="H10" s="17"/>
+      <c r="J10" s="14"/>
     </row>
     <row r="11" ht="14.25">
+      <c r="A11" s="13"/>
       <c r="B11" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>43</v>
@@ -3419,13 +3506,18 @@
         <v>67</v>
       </c>
       <c r="E11" t="s">
-        <v>174</v>
-      </c>
-      <c r="H11" s="12"/>
+        <v>176</v>
+      </c>
+      <c r="G11" s="15">
+        <v>44131</v>
+      </c>
+      <c r="H11" s="16"/>
+      <c r="J11" s="14"/>
     </row>
     <row r="12" ht="14.25">
+      <c r="A12" s="13"/>
       <c r="B12" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>43</v>
@@ -3434,13 +3526,18 @@
         <v>60</v>
       </c>
       <c r="E12" t="s">
-        <v>174</v>
-      </c>
-      <c r="H12" s="12"/>
+        <v>176</v>
+      </c>
+      <c r="G12" s="15">
+        <v>44049</v>
+      </c>
+      <c r="H12" s="16"/>
+      <c r="J12" s="14"/>
     </row>
     <row r="13" ht="14.25">
+      <c r="A13" s="18"/>
       <c r="B13" s="1" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>43</v>
@@ -3449,24 +3546,34 @@
         <v>38</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>174</v>
-      </c>
-      <c r="H13" s="12"/>
+        <v>176</v>
+      </c>
+      <c r="G13" s="15">
+        <v>43947</v>
+      </c>
+      <c r="H13" s="16"/>
+      <c r="J13" s="14"/>
     </row>
     <row r="14" ht="14.25">
+      <c r="A14" s="18"/>
       <c r="B14" s="1" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>43</v>
       </c>
       <c r="D14" s="1"/>
       <c r="E14" s="1"/>
-      <c r="H14" s="12"/>
+      <c r="G14" s="15">
+        <v>44173</v>
+      </c>
+      <c r="H14" s="16"/>
+      <c r="J14" s="14"/>
     </row>
     <row r="15" ht="14.25">
+      <c r="A15" s="18"/>
       <c r="B15" t="s">
-        <v>192</v>
+        <v>194</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>43</v>
@@ -3475,16 +3582,20 @@
         <v>20</v>
       </c>
       <c r="E15" t="s">
-        <v>174</v>
-      </c>
-      <c r="H15" s="12"/>
+        <v>176</v>
+      </c>
+      <c r="G15" s="15">
+        <v>44169</v>
+      </c>
+      <c r="H15" s="16"/>
+      <c r="J15" s="14"/>
     </row>
     <row r="16" ht="14.25">
       <c r="A16" t="s">
-        <v>193</v>
+        <v>195</v>
       </c>
       <c r="B16" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>63</v>
@@ -3493,25 +3604,34 @@
         <v>63</v>
       </c>
       <c r="E16" t="s">
-        <v>174</v>
-      </c>
-      <c r="H16" s="12"/>
+        <v>176</v>
+      </c>
+      <c r="G16" s="15">
+        <v>44166</v>
+      </c>
+      <c r="H16" s="16"/>
+      <c r="J16" s="14"/>
     </row>
     <row r="17" ht="14.25">
-      <c r="A17" s="1"/>
+      <c r="A17" s="13"/>
       <c r="B17" s="1" t="s">
-        <v>195</v>
+        <v>197</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>43</v>
       </c>
       <c r="D17" s="1"/>
       <c r="E17" s="1"/>
-      <c r="H17" s="12"/>
+      <c r="G17" s="15">
+        <v>44182</v>
+      </c>
+      <c r="H17" s="16"/>
+      <c r="J17" s="14"/>
     </row>
     <row r="18" ht="14.25">
+      <c r="A18" s="18"/>
       <c r="B18" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>43</v>
@@ -3520,13 +3640,18 @@
         <v>51</v>
       </c>
       <c r="E18" t="s">
-        <v>174</v>
-      </c>
-      <c r="H18" s="12"/>
+        <v>176</v>
+      </c>
+      <c r="G18" s="15">
+        <v>44177</v>
+      </c>
+      <c r="H18" s="16"/>
+      <c r="J18" s="14"/>
     </row>
     <row r="19" ht="14.25">
+      <c r="A19" s="18"/>
       <c r="B19" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>43</v>
@@ -3535,16 +3660,20 @@
         <v>64</v>
       </c>
       <c r="E19" t="s">
-        <v>171</v>
-      </c>
-      <c r="H19" s="12"/>
+        <v>173</v>
+      </c>
+      <c r="G19" s="15">
+        <v>44193</v>
+      </c>
+      <c r="H19" s="16"/>
+      <c r="J19" s="14"/>
     </row>
     <row r="20" ht="14.25">
       <c r="A20" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
       <c r="B20" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>63</v>
@@ -3553,13 +3682,18 @@
         <v>64</v>
       </c>
       <c r="E20" t="s">
-        <v>174</v>
-      </c>
-      <c r="H20" s="12"/>
+        <v>176</v>
+      </c>
+      <c r="G20" s="15">
+        <v>44174</v>
+      </c>
+      <c r="H20" s="16"/>
+      <c r="J20" s="14"/>
     </row>
     <row r="21" ht="14.25">
+      <c r="A21" s="13"/>
       <c r="B21" t="s">
-        <v>200</v>
+        <v>202</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>43</v>
@@ -3568,438 +3702,598 @@
         <v>63</v>
       </c>
       <c r="E21" t="s">
-        <v>174</v>
-      </c>
-      <c r="H21" s="12"/>
+        <v>176</v>
+      </c>
+      <c r="G21" s="15">
+        <v>44189</v>
+      </c>
+      <c r="H21" s="16"/>
+      <c r="J21" s="14"/>
     </row>
     <row r="22" ht="14.25">
       <c r="A22" t="s">
-        <v>201</v>
+        <v>203</v>
       </c>
       <c r="B22" t="s">
-        <v>202</v>
-      </c>
-      <c r="C22" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="C22" s="19" t="s">
         <v>63</v>
       </c>
       <c r="D22">
         <v>35</v>
       </c>
       <c r="E22" t="s">
-        <v>174</v>
-      </c>
-      <c r="H22" s="12"/>
+        <v>176</v>
+      </c>
+      <c r="G22" s="15">
+        <v>44164</v>
+      </c>
+      <c r="H22" s="16"/>
+      <c r="I22" s="19"/>
+      <c r="J22" s="20"/>
+      <c r="K22" s="19"/>
+      <c r="L22" s="19"/>
+      <c r="M22" s="19"/>
+      <c r="N22" s="19"/>
+      <c r="O22" s="19"/>
+      <c r="P22" s="19"/>
+      <c r="Q22" s="19"/>
+      <c r="R22" s="19"/>
     </row>
     <row r="23" ht="14.25">
       <c r="A23" t="s">
-        <v>203</v>
+        <v>205</v>
       </c>
       <c r="B23" t="s">
-        <v>204</v>
-      </c>
-      <c r="C23" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="C23" s="19" t="s">
         <v>63</v>
       </c>
       <c r="D23">
         <v>67</v>
       </c>
       <c r="E23" t="s">
-        <v>174</v>
-      </c>
-      <c r="H23" s="12"/>
+        <v>176</v>
+      </c>
+      <c r="G23" s="15">
+        <v>44165</v>
+      </c>
+      <c r="H23" s="16"/>
+      <c r="I23" s="19"/>
+      <c r="J23" s="20"/>
+      <c r="K23" s="19"/>
+      <c r="L23" s="19"/>
+      <c r="M23" s="19"/>
+      <c r="N23" s="19"/>
+      <c r="O23" s="19"/>
+      <c r="P23" s="19"/>
+      <c r="Q23" s="19"/>
+      <c r="R23" s="19"/>
     </row>
     <row r="24" ht="14.25">
+      <c r="A24" s="13"/>
       <c r="B24" t="s">
-        <v>205</v>
-      </c>
-      <c r="C24" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="C24" s="19" t="s">
         <v>43</v>
       </c>
       <c r="D24">
         <v>64</v>
       </c>
       <c r="E24" t="s">
-        <v>174</v>
-      </c>
-      <c r="H24" s="12"/>
+        <v>176</v>
+      </c>
+      <c r="G24" s="15">
+        <v>44164</v>
+      </c>
+      <c r="H24" s="16"/>
+      <c r="I24" s="19"/>
+      <c r="J24" s="20"/>
+      <c r="K24" s="19"/>
+      <c r="L24" s="19"/>
+      <c r="M24" s="19"/>
+      <c r="N24" s="19"/>
+      <c r="O24" s="19"/>
+      <c r="P24" s="19"/>
+      <c r="Q24" s="19"/>
+      <c r="R24" s="19"/>
     </row>
     <row r="25" ht="14.25">
-      <c r="B25" s="1" t="s">
-        <v>206</v>
-      </c>
-      <c r="C25" s="1" t="s">
+      <c r="A25" s="21"/>
+      <c r="B25" s="22" t="s">
+        <v>208</v>
+      </c>
+      <c r="C25" s="22" t="s">
         <v>63</v>
       </c>
-      <c r="D25" s="1">
+      <c r="D25" s="22">
         <v>76</v>
       </c>
-      <c r="E25" s="1" t="s">
-        <v>174</v>
-      </c>
-      <c r="H25" s="12"/>
+      <c r="E25" s="22" t="s">
+        <v>176</v>
+      </c>
+      <c r="F25" s="22"/>
+      <c r="G25" s="15">
+        <v>44165</v>
+      </c>
+      <c r="H25" s="16"/>
+      <c r="I25" s="22"/>
+      <c r="J25" s="23"/>
+      <c r="K25" s="22"/>
+      <c r="L25" s="22"/>
+      <c r="M25" s="22"/>
+      <c r="N25" s="22"/>
+      <c r="O25" s="22"/>
+      <c r="P25" s="22"/>
+      <c r="Q25" s="22"/>
+      <c r="R25" s="22"/>
+      <c r="S25" s="22"/>
+      <c r="T25" s="16"/>
     </row>
     <row r="26" ht="14.25">
-      <c r="B26" s="1" t="s">
-        <v>207</v>
-      </c>
-      <c r="E26" s="1"/>
-      <c r="H26" s="12"/>
+      <c r="A26" s="21"/>
+      <c r="B26" s="22" t="s">
+        <v>209</v>
+      </c>
+      <c r="C26" s="22"/>
+      <c r="D26" s="22"/>
+      <c r="E26" s="22"/>
+      <c r="F26" s="22"/>
+      <c r="G26" s="22"/>
+      <c r="H26" s="22"/>
+      <c r="I26" s="22"/>
+      <c r="J26" s="23"/>
+      <c r="K26" s="22"/>
+      <c r="L26" s="22"/>
+      <c r="M26" s="22"/>
+      <c r="N26" s="22"/>
+      <c r="O26" s="22"/>
+      <c r="P26" s="22"/>
+      <c r="Q26" s="22"/>
+      <c r="R26" s="22"/>
+      <c r="S26" s="22"/>
+      <c r="T26" s="16"/>
     </row>
     <row r="27" ht="14.25">
-      <c r="A27" s="13" t="s">
-        <v>208</v>
-      </c>
-      <c r="B27" s="13" t="s">
-        <v>209</v>
-      </c>
-      <c r="C27" s="13" t="s">
+      <c r="A27" s="24" t="s">
+        <v>210</v>
+      </c>
+      <c r="B27" s="24" t="s">
+        <v>211</v>
+      </c>
+      <c r="C27" s="24" t="s">
         <v>98</v>
       </c>
-      <c r="D27" s="13"/>
-      <c r="E27" s="13"/>
-      <c r="F27" s="13" t="s">
-        <v>210</v>
-      </c>
-      <c r="G27" s="13" t="s">
-        <v>211</v>
-      </c>
-      <c r="H27" s="14">
+      <c r="D27" s="24"/>
+      <c r="E27" s="24"/>
+      <c r="F27" s="24" t="s">
+        <v>212</v>
+      </c>
+      <c r="G27" s="25">
+        <f>K27</f>
         <v>44544</v>
       </c>
-      <c r="I27" s="14">
+      <c r="H27" s="24"/>
+      <c r="I27" s="24" t="s">
+        <v>213</v>
+      </c>
+      <c r="J27" s="26">
         <v>44544</v>
       </c>
-      <c r="J27" s="14">
+      <c r="K27" s="26">
+        <v>44544</v>
+      </c>
+      <c r="L27" s="26">
         <v>44566</v>
       </c>
-      <c r="K27" s="13">
+      <c r="M27" s="24">
         <v>144</v>
       </c>
-      <c r="L27" s="14">
+      <c r="N27" s="26">
         <v>44557</v>
       </c>
-      <c r="M27" s="14">
+      <c r="O27" s="26">
         <v>44594</v>
       </c>
-      <c r="N27" s="14">
+      <c r="P27" s="26">
         <v>44567</v>
       </c>
-      <c r="O27" s="14">
+      <c r="Q27" s="26">
         <v>44588</v>
       </c>
-      <c r="P27" s="14">
+      <c r="R27" s="26">
         <v>44596</v>
       </c>
+      <c r="S27" s="22"/>
+      <c r="T27" s="16"/>
     </row>
     <row r="28" ht="14.25">
-      <c r="A28" s="15" t="s">
+      <c r="A28" s="27" t="s">
+        <v>214</v>
+      </c>
+      <c r="B28" s="27" t="s">
+        <v>215</v>
+      </c>
+      <c r="C28" s="27" t="s">
+        <v>98</v>
+      </c>
+      <c r="D28" s="27"/>
+      <c r="E28" s="27"/>
+      <c r="F28" s="27"/>
+      <c r="G28" s="28">
+        <f>K28</f>
+        <v>44547</v>
+      </c>
+      <c r="H28" s="27"/>
+      <c r="I28" s="27" t="s">
+        <v>213</v>
+      </c>
+      <c r="J28" s="29">
+        <v>44547</v>
+      </c>
+      <c r="K28" s="29">
+        <v>44547</v>
+      </c>
+      <c r="L28" s="29">
+        <v>44563</v>
+      </c>
+      <c r="M28" s="27">
+        <v>144</v>
+      </c>
+      <c r="N28" s="29">
+        <v>44547</v>
+      </c>
+      <c r="O28" s="29"/>
+      <c r="P28" s="29">
+        <v>44564</v>
+      </c>
+      <c r="Q28" s="29">
+        <v>44616</v>
+      </c>
+      <c r="R28" s="27"/>
+      <c r="S28" s="22"/>
+      <c r="T28" s="16"/>
+    </row>
+    <row r="29" ht="14.25">
+      <c r="A29" s="30" t="s">
+        <v>216</v>
+      </c>
+      <c r="B29" s="30" t="s">
+        <v>217</v>
+      </c>
+      <c r="C29" s="30" t="s">
+        <v>98</v>
+      </c>
+      <c r="D29" s="30"/>
+      <c r="E29" s="30"/>
+      <c r="F29" s="30" t="s">
+        <v>218</v>
+      </c>
+      <c r="G29" s="25">
+        <f>K29</f>
+        <v>44564</v>
+      </c>
+      <c r="H29" s="30"/>
+      <c r="I29" s="30" t="s">
+        <v>213</v>
+      </c>
+      <c r="J29" s="31">
+        <v>44564</v>
+      </c>
+      <c r="K29" s="31">
+        <v>44564</v>
+      </c>
+      <c r="L29" s="31">
+        <v>44573</v>
+      </c>
+      <c r="M29" s="30">
+        <v>144</v>
+      </c>
+      <c r="N29" s="31">
+        <v>44570</v>
+      </c>
+      <c r="O29" s="31"/>
+      <c r="P29" s="31">
+        <v>44573</v>
+      </c>
+      <c r="Q29" s="31"/>
+      <c r="R29" s="31">
+        <v>44584</v>
+      </c>
+      <c r="S29" s="22"/>
+      <c r="T29" s="16"/>
+    </row>
+    <row r="30" ht="14.25">
+      <c r="A30" s="30" t="s">
+        <v>219</v>
+      </c>
+      <c r="B30" s="30" t="s">
+        <v>220</v>
+      </c>
+      <c r="C30" s="30" t="s">
+        <v>98</v>
+      </c>
+      <c r="D30" s="30"/>
+      <c r="E30" s="30"/>
+      <c r="F30" s="30" t="s">
+        <v>218</v>
+      </c>
+      <c r="G30" s="28">
+        <f>K30</f>
+        <v>44563</v>
+      </c>
+      <c r="H30" s="30"/>
+      <c r="I30" s="30" t="s">
+        <v>213</v>
+      </c>
+      <c r="J30" s="31">
+        <v>44560</v>
+      </c>
+      <c r="K30" s="31">
+        <v>44563</v>
+      </c>
+      <c r="L30" s="31">
+        <v>44577</v>
+      </c>
+      <c r="M30" s="30">
+        <v>144</v>
+      </c>
+      <c r="N30" s="31">
+        <v>44563</v>
+      </c>
+      <c r="O30" s="31"/>
+      <c r="P30" s="31">
+        <v>44563</v>
+      </c>
+      <c r="Q30" s="31"/>
+      <c r="R30" s="31">
+        <v>44616</v>
+      </c>
+      <c r="S30" s="22"/>
+      <c r="T30" s="16"/>
+    </row>
+    <row r="31" ht="14.25">
+      <c r="A31" s="24" t="s">
+        <v>221</v>
+      </c>
+      <c r="B31" s="24" t="s">
+        <v>222</v>
+      </c>
+      <c r="C31" s="24" t="s">
+        <v>98</v>
+      </c>
+      <c r="D31" s="24"/>
+      <c r="E31" s="24"/>
+      <c r="F31" s="24" t="s">
         <v>212</v>
       </c>
-      <c r="B28" s="15" t="s">
+      <c r="G31" s="25">
+        <f>K31</f>
+        <v>44569</v>
+      </c>
+      <c r="H31" s="24"/>
+      <c r="I31" s="24" t="s">
         <v>213</v>
       </c>
-      <c r="C28" s="15" t="s">
+      <c r="J31" s="26">
+        <v>44564</v>
+      </c>
+      <c r="K31" s="26">
+        <v>44569</v>
+      </c>
+      <c r="L31" s="26">
+        <v>44585</v>
+      </c>
+      <c r="M31" s="24">
+        <v>144</v>
+      </c>
+      <c r="N31" s="26">
+        <v>44569</v>
+      </c>
+      <c r="O31" s="26">
+        <v>44633</v>
+      </c>
+      <c r="P31" s="26">
+        <v>44585</v>
+      </c>
+      <c r="Q31" s="26">
+        <v>44630</v>
+      </c>
+      <c r="R31" s="26">
+        <v>44636</v>
+      </c>
+      <c r="S31" s="22"/>
+      <c r="T31" s="16"/>
+    </row>
+    <row r="32" ht="14.25">
+      <c r="A32" s="30" t="s">
+        <v>223</v>
+      </c>
+      <c r="B32" s="30" t="s">
+        <v>224</v>
+      </c>
+      <c r="C32" s="30" t="s">
         <v>98</v>
       </c>
-      <c r="D28" s="15"/>
-      <c r="E28" s="15"/>
-      <c r="F28" s="15" t="s">
-        <v>214</v>
-      </c>
-      <c r="G28" s="15" t="s">
-        <v>211</v>
-      </c>
-      <c r="H28" s="16">
-        <v>44547</v>
-      </c>
-      <c r="I28" s="16">
-        <v>44547</v>
-      </c>
-      <c r="J28" s="16">
-        <v>44563</v>
-      </c>
-      <c r="K28" s="15">
+      <c r="D32" s="30"/>
+      <c r="E32" s="30"/>
+      <c r="F32" s="30" t="s">
+        <v>218</v>
+      </c>
+      <c r="G32" s="28">
+        <f>K32</f>
+        <v>44576</v>
+      </c>
+      <c r="H32" s="30"/>
+      <c r="I32" s="30"/>
+      <c r="J32" s="31">
+        <v>44569</v>
+      </c>
+      <c r="K32" s="31">
+        <v>44576</v>
+      </c>
+      <c r="L32" s="31">
+        <v>44599</v>
+      </c>
+      <c r="M32" s="30">
         <v>144</v>
       </c>
-      <c r="L28" s="16">
-        <v>44547</v>
-      </c>
-      <c r="M28" s="16"/>
-      <c r="N28" s="16">
-        <v>44564</v>
-      </c>
-      <c r="O28" s="16">
-        <v>44616</v>
-      </c>
-      <c r="P28" s="15"/>
-    </row>
-    <row r="29" ht="14.25">
-      <c r="A29" s="17" t="s">
-        <v>215</v>
-      </c>
-      <c r="B29" s="17" t="s">
-        <v>216</v>
-      </c>
-      <c r="C29" s="17" t="s">
+      <c r="N32" s="31">
+        <v>44578</v>
+      </c>
+      <c r="O32" s="31"/>
+      <c r="P32" s="31">
+        <v>44599</v>
+      </c>
+      <c r="Q32" s="31"/>
+      <c r="R32" s="31">
+        <v>44621</v>
+      </c>
+      <c r="S32" s="22"/>
+      <c r="T32" s="16"/>
+    </row>
+    <row r="33" ht="14.25">
+      <c r="A33" s="24" t="s">
+        <v>225</v>
+      </c>
+      <c r="B33" s="24" t="s">
+        <v>226</v>
+      </c>
+      <c r="C33" s="24" t="s">
         <v>98</v>
       </c>
-      <c r="D29" s="17"/>
-      <c r="E29" s="17"/>
-      <c r="F29" s="17" t="s">
-        <v>217</v>
-      </c>
-      <c r="G29" s="17" t="s">
-        <v>211</v>
-      </c>
-      <c r="H29" s="18">
-        <v>44564</v>
-      </c>
-      <c r="I29" s="18">
-        <v>44564</v>
-      </c>
-      <c r="J29" s="18">
-        <v>44573</v>
-      </c>
-      <c r="K29" s="17">
+      <c r="D33" s="24"/>
+      <c r="E33" s="24"/>
+      <c r="F33" s="24" t="s">
+        <v>212</v>
+      </c>
+      <c r="G33" s="25">
+        <f>K33</f>
+        <v>44585</v>
+      </c>
+      <c r="H33" s="24"/>
+      <c r="I33" s="24"/>
+      <c r="J33" s="26">
+        <v>44585</v>
+      </c>
+      <c r="K33" s="26">
+        <v>44585</v>
+      </c>
+      <c r="L33" s="26">
+        <v>44597</v>
+      </c>
+      <c r="M33" s="24">
         <v>144</v>
       </c>
-      <c r="L29" s="18">
-        <v>44570</v>
-      </c>
-      <c r="M29" s="18" t="s">
+      <c r="N33" s="26">
+        <v>44585</v>
+      </c>
+      <c r="O33" s="26">
+        <v>44658</v>
+      </c>
+      <c r="P33" s="26">
+        <v>44597</v>
+      </c>
+      <c r="Q33" s="26">
+        <v>44653</v>
+      </c>
+      <c r="R33" s="24"/>
+      <c r="S33" s="22"/>
+      <c r="T33" s="16"/>
+    </row>
+    <row r="34" ht="14.25">
+      <c r="A34" s="30" t="s">
+        <v>227</v>
+      </c>
+      <c r="B34" s="30" t="s">
+        <v>228</v>
+      </c>
+      <c r="C34" s="30" t="s">
+        <v>98</v>
+      </c>
+      <c r="D34" s="30"/>
+      <c r="E34" s="30"/>
+      <c r="F34" s="30" t="s">
         <v>218</v>
       </c>
-      <c r="N29" s="18">
-        <v>44573</v>
-      </c>
-      <c r="O29" s="18" t="s">
-        <v>218</v>
-      </c>
-      <c r="P29" s="18">
-        <v>44584</v>
-      </c>
-    </row>
-    <row r="30" ht="14.25">
-      <c r="A30" s="17" t="s">
-        <v>219</v>
-      </c>
-      <c r="B30" s="17" t="s">
-        <v>220</v>
-      </c>
-      <c r="C30" s="17" t="s">
-        <v>98</v>
-      </c>
-      <c r="D30" s="17"/>
-      <c r="E30" s="17"/>
-      <c r="F30" s="17" t="s">
-        <v>217</v>
-      </c>
-      <c r="G30" s="17" t="s">
-        <v>211</v>
-      </c>
-      <c r="H30" s="18">
-        <v>44560</v>
-      </c>
-      <c r="I30" s="18">
-        <v>44563</v>
-      </c>
-      <c r="J30" s="18">
-        <v>44577</v>
-      </c>
-      <c r="K30" s="17">
+      <c r="G34" s="28">
+        <f>K34</f>
+        <v>44607</v>
+      </c>
+      <c r="H34" s="30"/>
+      <c r="I34" s="30"/>
+      <c r="J34" s="31">
+        <v>44607</v>
+      </c>
+      <c r="K34" s="31">
+        <v>44607</v>
+      </c>
+      <c r="L34" s="31">
+        <v>44612</v>
+      </c>
+      <c r="M34" s="30">
         <v>144</v>
       </c>
-      <c r="L30" s="18">
-        <v>44563</v>
-      </c>
-      <c r="M30" s="18" t="s">
-        <v>218</v>
-      </c>
-      <c r="N30" s="18">
-        <v>44563</v>
-      </c>
-      <c r="O30" s="18" t="s">
-        <v>218</v>
-      </c>
-      <c r="P30" s="18">
-        <v>44616</v>
-      </c>
-    </row>
-    <row r="31" ht="14.25">
-      <c r="A31" s="13" t="s">
-        <v>221</v>
-      </c>
-      <c r="B31" s="13" t="s">
-        <v>222</v>
-      </c>
-      <c r="C31" s="13" t="s">
-        <v>98</v>
-      </c>
-      <c r="D31" s="13"/>
-      <c r="E31" s="13"/>
-      <c r="F31" s="13" t="s">
-        <v>210</v>
-      </c>
-      <c r="G31" s="13" t="s">
-        <v>211</v>
-      </c>
-      <c r="H31" s="14">
-        <v>44564</v>
-      </c>
-      <c r="I31" s="14">
-        <v>44569</v>
-      </c>
-      <c r="J31" s="14">
-        <v>44585</v>
-      </c>
-      <c r="K31" s="13">
-        <v>144</v>
-      </c>
-      <c r="L31" s="14">
-        <v>44569</v>
-      </c>
-      <c r="M31" s="14">
-        <v>44633</v>
-      </c>
-      <c r="N31" s="14">
-        <v>44585</v>
-      </c>
-      <c r="O31" s="14">
-        <v>44630</v>
-      </c>
-      <c r="P31" s="14">
-        <v>44636</v>
-      </c>
-    </row>
-    <row r="32" ht="14.25">
-      <c r="A32" s="17" t="s">
-        <v>223</v>
-      </c>
-      <c r="B32" s="17" t="s">
-        <v>224</v>
-      </c>
-      <c r="C32" s="17" t="s">
-        <v>98</v>
-      </c>
-      <c r="D32" s="17"/>
-      <c r="E32" s="17"/>
-      <c r="F32" s="17" t="s">
-        <v>217</v>
-      </c>
-      <c r="G32" s="17"/>
-      <c r="H32" s="18">
-        <v>44569</v>
-      </c>
-      <c r="I32" s="18">
-        <v>44576</v>
-      </c>
-      <c r="J32" s="18">
-        <v>44599</v>
-      </c>
-      <c r="K32" s="17">
-        <v>144</v>
-      </c>
-      <c r="L32" s="18">
-        <v>44578</v>
-      </c>
-      <c r="M32" s="18" t="s">
-        <v>218</v>
-      </c>
-      <c r="N32" s="18">
-        <v>44599</v>
-      </c>
-      <c r="O32" s="18" t="s">
-        <v>218</v>
-      </c>
-      <c r="P32" s="18">
-        <v>44621</v>
-      </c>
-    </row>
-    <row r="33" ht="14.25">
-      <c r="A33" s="13" t="s">
-        <v>225</v>
-      </c>
-      <c r="B33" s="13" t="s">
-        <v>226</v>
-      </c>
-      <c r="C33" s="13" t="s">
-        <v>98</v>
-      </c>
-      <c r="D33" s="13"/>
-      <c r="E33" s="13"/>
-      <c r="F33" s="13" t="s">
-        <v>210</v>
-      </c>
-      <c r="G33" s="13"/>
-      <c r="H33" s="14">
-        <v>44585</v>
-      </c>
-      <c r="I33" s="14">
-        <v>44585</v>
-      </c>
-      <c r="J33" s="14">
-        <v>44597</v>
-      </c>
-      <c r="K33" s="13">
-        <v>144</v>
-      </c>
-      <c r="L33" s="14">
-        <v>44585</v>
-      </c>
-      <c r="M33" s="14">
-        <v>44658</v>
-      </c>
-      <c r="N33" s="14">
-        <v>44597</v>
-      </c>
-      <c r="O33" s="14">
-        <v>44653</v>
-      </c>
-      <c r="P33" s="13"/>
-    </row>
-    <row r="34" ht="14.25">
-      <c r="A34" s="17" t="s">
-        <v>227</v>
-      </c>
-      <c r="B34" s="17" t="s">
-        <v>228</v>
-      </c>
-      <c r="C34" s="17" t="s">
-        <v>98</v>
-      </c>
-      <c r="D34" s="17"/>
-      <c r="E34" s="17"/>
-      <c r="F34" s="17" t="s">
-        <v>217</v>
-      </c>
-      <c r="G34" s="17"/>
-      <c r="H34" s="18">
-        <v>44607</v>
-      </c>
-      <c r="I34" s="18">
-        <v>44607</v>
-      </c>
-      <c r="J34" s="18">
-        <v>44612</v>
-      </c>
-      <c r="K34" s="17">
-        <v>144</v>
-      </c>
-      <c r="L34" s="18">
+      <c r="N34" s="31">
         <v>44608</v>
       </c>
-      <c r="M34" s="18" t="s">
-        <v>218</v>
-      </c>
-      <c r="N34" s="18">
+      <c r="O34" s="31"/>
+      <c r="P34" s="31">
         <v>44613</v>
       </c>
-      <c r="O34" s="18" t="s">
-        <v>218</v>
-      </c>
-      <c r="P34" s="18">
+      <c r="Q34" s="31"/>
+      <c r="R34" s="31">
         <v>44641</v>
       </c>
+      <c r="S34" s="22"/>
+      <c r="T34" s="16"/>
+    </row>
+    <row r="35" ht="14.25">
+      <c r="A35" s="22"/>
+      <c r="B35" s="22"/>
+      <c r="C35" s="22"/>
+      <c r="D35" s="22"/>
+      <c r="E35" s="22"/>
+      <c r="F35" s="22"/>
+      <c r="G35" s="22"/>
+      <c r="H35" s="22"/>
+      <c r="I35" s="22"/>
+      <c r="J35" s="22"/>
+      <c r="K35" s="22"/>
+      <c r="L35" s="22"/>
+      <c r="M35" s="22"/>
+      <c r="N35" s="22"/>
+      <c r="O35" s="22"/>
+      <c r="P35" s="22"/>
+      <c r="Q35" s="22"/>
+      <c r="R35" s="22"/>
+      <c r="S35" s="22"/>
+      <c r="T35" s="16"/>
+    </row>
+    <row r="36" ht="14.25">
+      <c r="A36" s="16"/>
+      <c r="B36" s="16"/>
+      <c r="C36" s="16"/>
+      <c r="D36" s="16"/>
+      <c r="E36" s="16"/>
+      <c r="F36" s="16"/>
+      <c r="G36" s="16"/>
+      <c r="H36" s="16"/>
+      <c r="I36" s="16"/>
+      <c r="J36" s="16"/>
+      <c r="K36" s="16"/>
+      <c r="L36" s="16"/>
+      <c r="M36" s="16"/>
+      <c r="N36" s="16"/>
+      <c r="O36" s="16"/>
+      <c r="P36" s="16"/>
+      <c r="Q36" s="16"/>
+      <c r="R36" s="16"/>
+      <c r="S36" s="16"/>
+      <c r="T36" s="16"/>
     </row>
   </sheetData>
   <printOptions headings="0" gridLines="0"/>
@@ -4033,8 +4327,7 @@
     <col customWidth="1" min="9" max="9" style="0" width="10.630000000000001"/>
     <col customWidth="1" min="10" max="10" style="0" width="8.4000000000000004"/>
     <col customWidth="1" min="11" max="11" style="0" width="7.2800000000000002"/>
-    <col bestFit="1" customWidth="1" min="12" max="12" style="0" width="10.421875"/>
-    <col customWidth="1" min="13" max="13" style="0" width="9.2400000000000002"/>
+    <col bestFit="1" customWidth="1" min="12" max="13" style="0" width="10.421875"/>
     <col customWidth="1" min="14" max="14" style="0" width="9.6500000000000004"/>
     <col customWidth="1" min="15" max="15" style="0" width="8.2599999999999998"/>
     <col customWidth="1" min="16" max="16" style="0" width="7.8499999999999996"/>
@@ -4162,7 +4455,7 @@
         <v>254</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="G2" s="3">
         <v>14</v>
@@ -4172,13 +4465,14 @@
       </c>
       <c r="I2" s="3"/>
       <c r="J2" s="3"/>
-      <c r="K2" s="20" t="b">
+      <c r="K2" s="32" t="b">
         <f t="shared" ref="K2:K10" si="6">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="L2" s="12">
+      <c r="L2" s="14">
         <v>43927</v>
       </c>
+      <c r="M2" s="1"/>
       <c r="N2" s="1"/>
       <c r="O2" s="1"/>
       <c r="P2" s="1"/>
@@ -4198,7 +4492,7 @@
         <v>254</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="G3" s="3">
         <v>14</v>
@@ -4212,13 +4506,14 @@
       <c r="J3" s="3" t="s">
         <v>256</v>
       </c>
-      <c r="K3" s="20" t="b">
+      <c r="K3" s="32" t="b">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="L3" s="12">
+      <c r="L3" s="14">
         <v>43930</v>
       </c>
+      <c r="M3" s="1"/>
       <c r="N3" s="1"/>
       <c r="O3" s="1"/>
       <c r="P3" s="1"/>
@@ -4238,7 +4533,7 @@
         <v>254</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="G4" s="4">
         <v>7</v>
@@ -4256,9 +4551,10 @@
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="L4" s="12">
+      <c r="L4" s="14">
         <v>43936</v>
       </c>
+      <c r="M4" s="1"/>
       <c r="N4" s="1"/>
       <c r="O4" s="1"/>
       <c r="P4" s="1"/>
@@ -4278,7 +4574,7 @@
         <v>254</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="G5" s="4">
         <v>14</v>
@@ -4296,9 +4592,10 @@
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="L5" s="12">
+      <c r="L5" s="14">
         <v>43937</v>
       </c>
+      <c r="M5" s="1"/>
       <c r="N5" s="1"/>
       <c r="O5" s="1"/>
       <c r="P5" s="1"/>
@@ -4318,7 +4615,7 @@
         <v>254</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="G6" s="4">
         <v>25</v>
@@ -4336,9 +4633,10 @@
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="L6" s="12">
+      <c r="L6" s="14">
         <v>43938</v>
       </c>
+      <c r="M6" s="1"/>
       <c r="N6" s="1"/>
       <c r="O6" s="1"/>
       <c r="P6" s="1"/>
@@ -4358,7 +4656,7 @@
         <v>254</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="G7" s="4">
         <v>7</v>
@@ -4376,7 +4674,7 @@
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="L7" s="12">
+      <c r="L7" s="14">
         <v>43941</v>
       </c>
       <c r="M7" s="1"/>
@@ -4399,7 +4697,7 @@
         <v>254</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="G8" s="5">
         <v>25</v>
@@ -4417,7 +4715,7 @@
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="L8" s="12">
+      <c r="L8" s="14">
         <v>43950</v>
       </c>
       <c r="M8" s="1"/>
@@ -4440,7 +4738,7 @@
         <v>254</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="G9" s="5">
         <v>10</v>
@@ -4458,7 +4756,7 @@
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="L9" s="12">
+      <c r="L9" s="14">
         <v>43951</v>
       </c>
       <c r="M9" s="1"/>
@@ -4480,8 +4778,8 @@
       <c r="E10" s="6" t="s">
         <v>254</v>
       </c>
-      <c r="F10" s="21" t="s">
-        <v>187</v>
+      <c r="F10" s="33" t="s">
+        <v>189</v>
       </c>
       <c r="G10" s="6">
         <v>12</v>
@@ -4499,7 +4797,7 @@
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="L10" s="12">
+      <c r="L10" s="14">
         <v>43991</v>
       </c>
       <c r="M10" s="1"/>
@@ -4522,7 +4820,7 @@
         <v>254</v>
       </c>
       <c r="F11" s="7" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
       <c r="G11" s="7">
         <v>34</v>
@@ -4536,7 +4834,7 @@
         <f t="shared" ref="K11:K12" si="7">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="L11" s="12">
+      <c r="L11" s="14">
         <v>44165</v>
       </c>
       <c r="M11" s="1"/>
@@ -4559,7 +4857,7 @@
         <v>254</v>
       </c>
       <c r="F12" s="7" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="G12" s="7">
         <v>116</v>
@@ -4573,7 +4871,7 @@
         <f t="shared" si="7"/>
         <v>1</v>
       </c>
-      <c r="L12" s="12">
+      <c r="L12" s="14">
         <v>44165</v>
       </c>
       <c r="M12" s="1"/>
@@ -4596,7 +4894,7 @@
         <v>254</v>
       </c>
       <c r="F13" s="7" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="G13" s="7">
         <v>226</v>
@@ -4610,7 +4908,7 @@
         <f t="shared" ref="K13:K26" si="8">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="L13" s="12">
+      <c r="L13" s="14">
         <v>44173</v>
       </c>
       <c r="M13" s="1"/>
@@ -4633,7 +4931,7 @@
         <v>254</v>
       </c>
       <c r="F14" s="7" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
       <c r="G14" s="7"/>
       <c r="H14" s="7" t="s">
@@ -4647,9 +4945,7 @@
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="L14" s="12">
-        <v>44173</v>
-      </c>
+      <c r="L14" s="14"/>
       <c r="M14" s="1"/>
       <c r="N14" s="1"/>
       <c r="O14" s="1"/>
@@ -4670,7 +4966,7 @@
         <v>254</v>
       </c>
       <c r="F15" s="7" t="s">
-        <v>192</v>
+        <v>194</v>
       </c>
       <c r="G15" s="7">
         <v>6</v>
@@ -4684,7 +4980,7 @@
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="L15" s="12">
+      <c r="L15" s="14">
         <v>44175</v>
       </c>
       <c r="M15" s="1"/>
@@ -4707,7 +5003,7 @@
         <v>254</v>
       </c>
       <c r="F16" s="8" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
       <c r="G16" s="8">
         <v>15</v>
@@ -4721,7 +5017,7 @@
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="L16" s="12">
+      <c r="L16" s="14">
         <v>44181</v>
       </c>
       <c r="M16" s="1"/>
@@ -4744,7 +5040,7 @@
         <v>254</v>
       </c>
       <c r="F17" s="8" t="s">
-        <v>195</v>
+        <v>197</v>
       </c>
       <c r="G17" s="8"/>
       <c r="H17" s="8" t="s">
@@ -4758,9 +5054,7 @@
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="L17" s="12">
-        <v>44182</v>
-      </c>
+      <c r="L17" s="14"/>
       <c r="M17" s="1"/>
       <c r="N17" s="1"/>
       <c r="O17" s="1"/>
@@ -4781,7 +5075,7 @@
         <v>254</v>
       </c>
       <c r="F18" s="8" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="G18" s="8">
         <v>39</v>
@@ -4795,10 +5089,11 @@
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="L18" s="12">
+      <c r="L18" s="14">
         <v>44216</v>
       </c>
       <c r="M18" s="1"/>
+      <c r="N18" s="1"/>
       <c r="O18" s="1"/>
       <c r="P18" s="1"/>
     </row>
@@ -4817,7 +5112,7 @@
         <v>254</v>
       </c>
       <c r="F19" s="8" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
       <c r="G19" s="8">
         <v>23</v>
@@ -4831,10 +5126,12 @@
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="L19" s="12">
+      <c r="L19" s="14">
         <v>44216</v>
       </c>
       <c r="M19" s="1"/>
+      <c r="N19" s="1"/>
+      <c r="O19" s="1"/>
     </row>
     <row r="20" ht="14.25">
       <c r="A20" s="8" t="s">
@@ -4851,7 +5148,7 @@
         <v>254</v>
       </c>
       <c r="F20" s="8" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="G20" s="8">
         <v>43</v>
@@ -4865,10 +5162,12 @@
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="L20" s="12">
+      <c r="L20" s="14">
         <v>44217</v>
       </c>
       <c r="M20" s="1"/>
+      <c r="N20" s="1"/>
+      <c r="O20" s="1"/>
     </row>
     <row r="21" ht="14.25">
       <c r="A21" s="8" t="s">
@@ -4885,7 +5184,7 @@
         <v>254</v>
       </c>
       <c r="F21" s="8" t="s">
-        <v>200</v>
+        <v>202</v>
       </c>
       <c r="G21" s="8">
         <v>28</v>
@@ -4899,10 +5198,12 @@
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="L21" s="12">
+      <c r="L21" s="14">
         <v>44217</v>
       </c>
       <c r="M21" s="1"/>
+      <c r="N21" s="1"/>
+      <c r="O21" s="1"/>
     </row>
     <row r="22" ht="14.25">
       <c r="A22" s="8" t="s">
@@ -4919,7 +5220,7 @@
         <v>254</v>
       </c>
       <c r="F22" s="8" t="s">
-        <v>202</v>
+        <v>204</v>
       </c>
       <c r="G22" s="8">
         <v>54</v>
@@ -4933,10 +5234,12 @@
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="L22" s="12">
+      <c r="L22" s="14">
         <v>44218</v>
       </c>
       <c r="M22" s="1"/>
+      <c r="N22" s="1"/>
+      <c r="O22" s="1"/>
     </row>
     <row r="23" ht="14.25">
       <c r="A23" s="8" t="s">
@@ -4953,7 +5256,7 @@
         <v>254</v>
       </c>
       <c r="F23" s="8" t="s">
-        <v>204</v>
+        <v>206</v>
       </c>
       <c r="G23" s="8">
         <v>53</v>
@@ -4967,10 +5270,12 @@
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="L23" s="12">
+      <c r="L23" s="14">
         <v>44218</v>
       </c>
       <c r="M23" s="1"/>
+      <c r="N23" s="1"/>
+      <c r="O23" s="1"/>
     </row>
     <row r="24" ht="14.25">
       <c r="A24" s="8" t="s">
@@ -4987,7 +5292,7 @@
         <v>254</v>
       </c>
       <c r="F24" s="8" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
       <c r="G24" s="8">
         <v>54</v>
@@ -5001,10 +5306,12 @@
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="L24" s="12">
+      <c r="L24" s="14">
         <v>44218</v>
       </c>
       <c r="M24" s="1"/>
+      <c r="N24" s="1"/>
+      <c r="O24" s="1"/>
     </row>
     <row r="25" ht="14.25">
       <c r="A25" s="8" t="s">
@@ -5021,7 +5328,7 @@
         <v>254</v>
       </c>
       <c r="F25" s="8" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="G25" s="8">
         <v>65</v>
@@ -5035,10 +5342,12 @@
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="L25" s="12">
+      <c r="L25" s="14">
         <v>44230</v>
       </c>
       <c r="M25" s="1"/>
+      <c r="N25" s="1"/>
+      <c r="O25" s="1"/>
     </row>
     <row r="26" s="1" customFormat="1" ht="14.25">
       <c r="A26" s="9" t="s">
@@ -5050,10 +5359,10 @@
       <c r="E26" s="9" t="s">
         <v>254</v>
       </c>
-      <c r="F26" s="22" t="s">
-        <v>207</v>
-      </c>
-      <c r="G26" s="23"/>
+      <c r="F26" s="34" t="s">
+        <v>209</v>
+      </c>
+      <c r="G26" s="35"/>
       <c r="H26" s="9" t="s">
         <v>261</v>
       </c>
@@ -5063,9 +5372,8 @@
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="L26" s="12">
-        <v>44503</v>
-      </c>
+      <c r="L26" s="14"/>
+      <c r="M26" s="15"/>
     </row>
     <row r="27" ht="14.25">
       <c r="A27" s="4" t="s">
@@ -5084,7 +5392,7 @@
         <v>254</v>
       </c>
       <c r="F27" s="4" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="G27" s="4"/>
       <c r="H27" s="4" t="s">
@@ -5093,10 +5401,10 @@
       <c r="I27" s="4"/>
       <c r="J27" s="4"/>
       <c r="K27" s="4"/>
-      <c r="L27" s="12">
+      <c r="L27" s="14">
         <v>44573</v>
       </c>
-      <c r="M27" s="24">
+      <c r="M27" s="36">
         <v>0.54166666666666696</v>
       </c>
       <c r="N27" s="1">
@@ -5161,7 +5469,7 @@
         <v>254</v>
       </c>
       <c r="F28" s="4" t="s">
-        <v>213</v>
+        <v>215</v>
       </c>
       <c r="G28" s="4"/>
       <c r="H28" s="4" t="s">
@@ -5170,10 +5478,10 @@
       <c r="I28" s="4"/>
       <c r="J28" s="4"/>
       <c r="K28" s="4"/>
-      <c r="L28" s="12">
+      <c r="L28" s="14">
         <v>44574</v>
       </c>
-      <c r="M28" s="24">
+      <c r="M28" s="36">
         <v>0.59375</v>
       </c>
       <c r="N28" s="1">
@@ -5240,7 +5548,7 @@
         <v>254</v>
       </c>
       <c r="F29" s="4" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="G29" s="4"/>
       <c r="H29" s="4" t="s">
@@ -5249,10 +5557,10 @@
       <c r="I29" s="4"/>
       <c r="J29" s="4"/>
       <c r="K29" s="4"/>
-      <c r="L29" s="12">
+      <c r="L29" s="14">
         <v>44575</v>
       </c>
-      <c r="M29" s="24">
+      <c r="M29" s="36">
         <v>0.70833333333333304</v>
       </c>
       <c r="N29" s="1">
@@ -5326,10 +5634,10 @@
       <c r="I30" s="4"/>
       <c r="J30" s="4"/>
       <c r="K30" s="4"/>
-      <c r="L30" s="12">
+      <c r="L30" s="14">
         <v>44581</v>
       </c>
-      <c r="M30" s="24">
+      <c r="M30" s="36">
         <v>0.60416666666666696</v>
       </c>
       <c r="N30" s="1">
@@ -5403,10 +5711,10 @@
       <c r="I31" s="4"/>
       <c r="J31" s="4"/>
       <c r="K31" s="4"/>
-      <c r="L31" s="12">
+      <c r="L31" s="14">
         <v>44587</v>
       </c>
-      <c r="M31" s="24">
+      <c r="M31" s="36">
         <v>0.47916666666666702</v>
       </c>
       <c r="N31" s="1">
@@ -5463,7 +5771,7 @@
         <v>254</v>
       </c>
       <c r="F32" s="4" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="G32" s="4"/>
       <c r="H32" s="4" t="s">
@@ -5472,10 +5780,10 @@
       <c r="I32" s="4"/>
       <c r="J32" s="4"/>
       <c r="K32" s="4"/>
-      <c r="L32" s="12">
+      <c r="L32" s="14">
         <v>44587</v>
       </c>
-      <c r="M32" s="24">
+      <c r="M32" s="36">
         <v>0.52083333333333304</v>
       </c>
       <c r="N32" s="1">
@@ -5532,7 +5840,7 @@
         <v>254</v>
       </c>
       <c r="F33" s="4" t="s">
-        <v>213</v>
+        <v>215</v>
       </c>
       <c r="G33" s="4"/>
       <c r="H33" s="4" t="s">
@@ -5541,10 +5849,10 @@
       <c r="I33" s="4"/>
       <c r="J33" s="4"/>
       <c r="K33" s="4"/>
-      <c r="L33" s="12">
+      <c r="L33" s="14">
         <v>44589</v>
       </c>
-      <c r="M33" s="24">
+      <c r="M33" s="36">
         <v>0.47916666666666702</v>
       </c>
       <c r="N33" s="1">
@@ -5618,10 +5926,10 @@
       <c r="I34" s="4"/>
       <c r="J34" s="4"/>
       <c r="K34" s="4"/>
-      <c r="L34" s="12">
+      <c r="L34" s="14">
         <v>44595</v>
       </c>
-      <c r="M34" s="24">
+      <c r="M34" s="36">
         <v>0.55208333333333304</v>
       </c>
       <c r="N34" s="1">
@@ -5693,10 +6001,10 @@
       <c r="I35" s="4"/>
       <c r="J35" s="4"/>
       <c r="K35" s="4"/>
-      <c r="L35" s="12">
+      <c r="L35" s="14">
         <v>44600</v>
       </c>
-      <c r="M35" s="24">
+      <c r="M35" s="36">
         <v>0.51041666666666696</v>
       </c>
       <c r="N35" s="1">
@@ -5770,10 +6078,10 @@
       <c r="I36" s="4"/>
       <c r="J36" s="4"/>
       <c r="K36" s="4"/>
-      <c r="L36" s="12">
+      <c r="L36" s="14">
         <v>44600</v>
       </c>
-      <c r="M36" s="24">
+      <c r="M36" s="36">
         <v>0.53125</v>
       </c>
       <c r="N36" s="1">
@@ -5838,7 +6146,7 @@
         <v>254</v>
       </c>
       <c r="F37" s="4" t="s">
-        <v>213</v>
+        <v>215</v>
       </c>
       <c r="G37" s="4"/>
       <c r="H37" s="4" t="s">
@@ -5847,10 +6155,10 @@
       <c r="I37" s="4"/>
       <c r="J37" s="4"/>
       <c r="K37" s="4"/>
-      <c r="L37" s="12">
+      <c r="L37" s="14">
         <v>44600</v>
       </c>
-      <c r="M37" s="24">
+      <c r="M37" s="36">
         <v>0.5625</v>
       </c>
       <c r="N37" s="1">
@@ -5924,10 +6232,10 @@
       <c r="I38" s="4"/>
       <c r="J38" s="4"/>
       <c r="K38" s="4"/>
-      <c r="L38" s="12">
+      <c r="L38" s="14">
         <v>44608</v>
       </c>
-      <c r="M38" s="24">
+      <c r="M38" s="36">
         <v>0.55208333333333304</v>
       </c>
       <c r="N38" s="1">
@@ -5997,7 +6305,7 @@
       <c r="I39" s="4"/>
       <c r="J39" s="4"/>
       <c r="K39" s="4"/>
-      <c r="L39" s="12">
+      <c r="L39" s="14">
         <v>44609</v>
       </c>
       <c r="M39" s="1"/>
@@ -6052,10 +6360,10 @@
       <c r="I40" s="4"/>
       <c r="J40" s="4"/>
       <c r="K40" s="4"/>
-      <c r="L40" s="12">
+      <c r="L40" s="14">
         <v>44615</v>
       </c>
-      <c r="M40" s="24">
+      <c r="M40" s="36">
         <v>0.625</v>
       </c>
       <c r="N40" s="1">
@@ -6127,10 +6435,10 @@
       <c r="I41" s="4"/>
       <c r="J41" s="4"/>
       <c r="K41" s="4"/>
-      <c r="L41" s="12">
+      <c r="L41" s="14">
         <v>44615</v>
       </c>
-      <c r="M41" s="24">
+      <c r="M41" s="36">
         <v>0.6875</v>
       </c>
       <c r="N41" s="1">
@@ -6202,10 +6510,10 @@
       <c r="I42" s="4"/>
       <c r="J42" s="4"/>
       <c r="K42" s="4"/>
-      <c r="L42" s="12">
+      <c r="L42" s="14">
         <v>44616</v>
       </c>
-      <c r="M42" s="24">
+      <c r="M42" s="36">
         <v>0.52083333333333304</v>
       </c>
       <c r="N42" s="1">
@@ -6264,7 +6572,7 @@
         <v>254</v>
       </c>
       <c r="F43" s="4" t="s">
-        <v>213</v>
+        <v>215</v>
       </c>
       <c r="G43" s="4"/>
       <c r="H43" s="4" t="s">
@@ -6273,10 +6581,10 @@
       <c r="I43" s="4"/>
       <c r="J43" s="4"/>
       <c r="K43" s="4"/>
-      <c r="L43" s="12">
+      <c r="L43" s="14">
         <v>44616</v>
       </c>
-      <c r="M43" s="24">
+      <c r="M43" s="36">
         <v>0.5625</v>
       </c>
       <c r="N43" s="1">
@@ -6348,10 +6656,10 @@
       <c r="I44" s="4"/>
       <c r="J44" s="4"/>
       <c r="K44" s="4"/>
-      <c r="L44" s="12">
+      <c r="L44" s="14">
         <v>44622</v>
       </c>
-      <c r="M44" s="24">
+      <c r="M44" s="36">
         <v>0.52083333333333304</v>
       </c>
       <c r="N44" s="1">
@@ -6423,10 +6731,10 @@
       <c r="I45" s="4"/>
       <c r="J45" s="4"/>
       <c r="K45" s="4"/>
-      <c r="L45" s="12">
+      <c r="L45" s="14">
         <v>44629</v>
       </c>
-      <c r="M45" s="24">
+      <c r="M45" s="36">
         <v>0.5</v>
       </c>
       <c r="N45" s="1">
@@ -6468,7 +6776,7 @@
       </c>
       <c r="AA45" s="1"/>
       <c r="AB45" s="1"/>
-      <c r="AC45" s="24">
+      <c r="AC45" s="36">
         <v>0.77777777777777801</v>
       </c>
       <c r="AD45" s="1"/>
@@ -6500,10 +6808,10 @@
       <c r="I46" s="4"/>
       <c r="J46" s="4"/>
       <c r="K46" s="4"/>
-      <c r="L46" s="12">
+      <c r="L46" s="14">
         <v>44629</v>
       </c>
-      <c r="M46" s="24">
+      <c r="M46" s="36">
         <v>0.53125</v>
       </c>
       <c r="N46" s="1">
@@ -6547,7 +6855,7 @@
       </c>
       <c r="AA46" s="1"/>
       <c r="AB46" s="1"/>
-      <c r="AC46" s="24">
+      <c r="AC46" s="36">
         <v>0.77777777777777801</v>
       </c>
       <c r="AD46" s="1"/>
@@ -6579,10 +6887,10 @@
       <c r="I47" s="4"/>
       <c r="J47" s="4"/>
       <c r="K47" s="4"/>
-      <c r="L47" s="12">
+      <c r="L47" s="14">
         <v>44637</v>
       </c>
-      <c r="M47" s="24">
+      <c r="M47" s="36">
         <v>0.52083333333333304</v>
       </c>
       <c r="N47" s="1">
@@ -6622,13 +6930,13 @@
       <c r="Z47" s="1">
         <v>0</v>
       </c>
-      <c r="AA47" s="24">
+      <c r="AA47" s="36">
         <v>0.56111111111111101</v>
       </c>
-      <c r="AB47" s="24">
+      <c r="AB47" s="36">
         <v>0.625</v>
       </c>
-      <c r="AC47" s="24">
+      <c r="AC47" s="36">
         <v>0.64375000000000004</v>
       </c>
       <c r="AD47" s="1"/>
@@ -6651,7 +6959,7 @@
         <v>254</v>
       </c>
       <c r="F48" s="4" t="s">
-        <v>213</v>
+        <v>215</v>
       </c>
       <c r="G48" s="4"/>
       <c r="H48" s="4" t="s">
@@ -6660,10 +6968,10 @@
       <c r="I48" s="4"/>
       <c r="J48" s="4"/>
       <c r="K48" s="4"/>
-      <c r="L48" s="12">
+      <c r="L48" s="14">
         <v>44648</v>
       </c>
-      <c r="M48" s="24">
+      <c r="M48" s="36">
         <v>0.51041666666666696</v>
       </c>
       <c r="N48" s="1">
@@ -6733,10 +7041,10 @@
       <c r="I49" s="4"/>
       <c r="J49" s="4"/>
       <c r="K49" s="4"/>
-      <c r="L49" s="12">
+      <c r="L49" s="14">
         <v>44651</v>
       </c>
-      <c r="M49" s="24">
+      <c r="M49" s="36">
         <v>0.5625</v>
       </c>
       <c r="N49" s="1">
@@ -6802,7 +7110,7 @@
       <c r="C1" t="s">
         <v>237</v>
       </c>
-      <c r="D1" s="12" t="s">
+      <c r="D1" s="14" t="s">
         <v>298</v>
       </c>
       <c r="E1" t="s">
@@ -6817,201 +7125,201 @@
     </row>
     <row r="2" ht="14.25">
       <c r="A2" s="8" t="s">
-        <v>208</v>
+        <v>210</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="C2" s="8" t="s">
         <v>302</v>
       </c>
-      <c r="D2" s="25">
+      <c r="D2" s="37">
         <v>44568</v>
       </c>
-      <c r="E2" s="25"/>
-      <c r="F2" s="25"/>
-      <c r="G2" s="25"/>
+      <c r="E2" s="37"/>
+      <c r="F2" s="37"/>
+      <c r="G2" s="37"/>
     </row>
     <row r="3" ht="14.25">
       <c r="A3" s="8" t="s">
-        <v>208</v>
+        <v>210</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="C3" s="8" t="s">
         <v>303</v>
       </c>
-      <c r="D3" s="25"/>
-      <c r="E3" s="25">
+      <c r="D3" s="37"/>
+      <c r="E3" s="37">
         <v>44573</v>
       </c>
-      <c r="F3" s="25">
+      <c r="F3" s="37">
         <v>44573</v>
       </c>
-      <c r="G3" s="25">
+      <c r="G3" s="37">
         <v>44573</v>
       </c>
-      <c r="I3" s="12"/>
+      <c r="I3" s="14"/>
     </row>
     <row r="4" ht="14.25">
       <c r="A4" s="8" t="s">
-        <v>208</v>
+        <v>210</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="C4" s="8" t="s">
         <v>304</v>
       </c>
-      <c r="D4" s="25">
+      <c r="D4" s="37">
         <v>44585</v>
       </c>
-      <c r="E4" s="25">
+      <c r="E4" s="37">
         <v>44587</v>
       </c>
-      <c r="F4" s="25">
+      <c r="F4" s="37">
         <v>44587</v>
       </c>
-      <c r="G4" s="25">
+      <c r="G4" s="37">
         <v>44588</v>
       </c>
     </row>
     <row r="5" ht="14.25">
       <c r="A5" s="5" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>213</v>
+        <v>215</v>
       </c>
       <c r="C5" s="5" t="s">
         <v>303</v>
       </c>
-      <c r="D5" s="26">
+      <c r="D5" s="38">
         <v>44574</v>
       </c>
-      <c r="E5" s="26">
+      <c r="E5" s="38">
         <v>44574</v>
       </c>
-      <c r="F5" s="26">
+      <c r="F5" s="38">
         <v>44574</v>
       </c>
-      <c r="G5" s="26">
+      <c r="G5" s="38">
         <v>44573</v>
       </c>
     </row>
     <row r="6" ht="14.25">
       <c r="A6" s="5" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>213</v>
+        <v>215</v>
       </c>
       <c r="C6" s="5" t="s">
         <v>304</v>
       </c>
-      <c r="D6" s="26">
+      <c r="D6" s="38">
         <v>44587</v>
       </c>
-      <c r="E6" s="26">
+      <c r="E6" s="38">
         <v>44589</v>
       </c>
-      <c r="F6" s="26">
+      <c r="F6" s="38">
         <v>44589</v>
       </c>
-      <c r="G6" s="26">
+      <c r="G6" s="38">
         <v>44588</v>
       </c>
     </row>
     <row r="7" ht="14.25">
       <c r="A7" s="5" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>213</v>
+        <v>215</v>
       </c>
       <c r="C7" s="5" t="s">
         <v>305</v>
       </c>
-      <c r="D7" s="26">
+      <c r="D7" s="38">
         <v>44601</v>
       </c>
-      <c r="E7" s="26">
+      <c r="E7" s="38">
         <v>44600</v>
       </c>
-      <c r="F7" s="26">
+      <c r="F7" s="38">
         <v>44600</v>
       </c>
-      <c r="G7" s="26">
+      <c r="G7" s="38">
         <v>44601</v>
       </c>
     </row>
     <row r="8" ht="14.25">
       <c r="A8" s="5" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>213</v>
+        <v>215</v>
       </c>
       <c r="C8" s="5" t="s">
         <v>306</v>
       </c>
-      <c r="D8" s="26">
+      <c r="D8" s="38">
         <v>44614</v>
       </c>
-      <c r="E8" s="26">
+      <c r="E8" s="38">
         <v>44616</v>
       </c>
-      <c r="F8" s="26">
+      <c r="F8" s="38">
         <v>44616</v>
       </c>
-      <c r="G8" s="26">
+      <c r="G8" s="38">
         <v>44617</v>
       </c>
     </row>
     <row r="9" ht="14.25">
       <c r="A9" s="5" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>213</v>
+        <v>215</v>
       </c>
       <c r="C9" s="5" t="s">
         <v>307</v>
       </c>
-      <c r="D9" s="26">
+      <c r="D9" s="38">
         <v>44645</v>
       </c>
-      <c r="E9" s="26">
+      <c r="E9" s="38">
         <v>44648</v>
       </c>
-      <c r="F9" s="26">
+      <c r="F9" s="38">
         <v>44648</v>
       </c>
-      <c r="G9" s="26">
+      <c r="G9" s="38">
         <v>44650</v>
       </c>
     </row>
     <row r="10" ht="14.25">
       <c r="A10" s="8" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="C10" s="8" t="s">
         <v>303</v>
       </c>
-      <c r="D10" s="25">
+      <c r="D10" s="37">
         <v>44575</v>
       </c>
-      <c r="E10" s="25">
+      <c r="E10" s="37">
         <v>44575</v>
       </c>
-      <c r="F10" s="25">
+      <c r="F10" s="37">
         <v>44575</v>
       </c>
-      <c r="G10" s="25">
+      <c r="G10" s="37">
         <v>44578</v>
       </c>
     </row>
@@ -7025,16 +7333,16 @@
       <c r="C11" s="5" t="s">
         <v>303</v>
       </c>
-      <c r="D11" s="26">
+      <c r="D11" s="38">
         <v>44581</v>
       </c>
-      <c r="E11" s="26">
+      <c r="E11" s="38">
         <v>44581</v>
       </c>
-      <c r="F11" s="26">
+      <c r="F11" s="38">
         <v>44581</v>
       </c>
-      <c r="G11" s="26">
+      <c r="G11" s="38">
         <v>44582</v>
       </c>
     </row>
@@ -7048,16 +7356,16 @@
       <c r="C12" s="5" t="s">
         <v>304</v>
       </c>
-      <c r="D12" s="26">
+      <c r="D12" s="38">
         <v>44594</v>
       </c>
-      <c r="E12" s="26">
+      <c r="E12" s="38">
         <v>44595</v>
       </c>
-      <c r="F12" s="26">
+      <c r="F12" s="38">
         <v>44595</v>
       </c>
-      <c r="G12" s="26">
+      <c r="G12" s="38">
         <v>44596</v>
       </c>
     </row>
@@ -7071,16 +7379,16 @@
       <c r="C13" s="5" t="s">
         <v>305</v>
       </c>
-      <c r="D13" s="26">
+      <c r="D13" s="38">
         <v>44609</v>
       </c>
-      <c r="E13" s="26">
+      <c r="E13" s="38">
         <v>44608</v>
       </c>
-      <c r="F13" s="26">
+      <c r="F13" s="38">
         <v>44608</v>
       </c>
-      <c r="G13" s="26">
+      <c r="G13" s="38">
         <v>44610</v>
       </c>
     </row>
@@ -7094,16 +7402,16 @@
       <c r="C14" s="8" t="s">
         <v>303</v>
       </c>
-      <c r="D14" s="25">
+      <c r="D14" s="37">
         <v>44585</v>
       </c>
-      <c r="E14" s="25">
+      <c r="E14" s="37">
         <v>44587</v>
       </c>
-      <c r="F14" s="25">
+      <c r="F14" s="37">
         <v>44587</v>
       </c>
-      <c r="G14" s="25">
+      <c r="G14" s="37">
         <v>44588</v>
       </c>
     </row>
@@ -7117,16 +7425,16 @@
       <c r="C15" s="8" t="s">
         <v>304</v>
       </c>
-      <c r="D15" s="25">
+      <c r="D15" s="37">
         <v>44600</v>
       </c>
-      <c r="E15" s="25">
+      <c r="E15" s="37">
         <v>44600</v>
       </c>
-      <c r="F15" s="25">
+      <c r="F15" s="37">
         <v>44600</v>
       </c>
-      <c r="G15" s="25">
+      <c r="G15" s="37">
         <v>44601</v>
       </c>
     </row>
@@ -7140,16 +7448,16 @@
       <c r="C16" s="8" t="s">
         <v>305</v>
       </c>
-      <c r="D16" s="25">
+      <c r="D16" s="37">
         <v>44615</v>
       </c>
-      <c r="E16" s="25">
+      <c r="E16" s="37">
         <v>44615</v>
       </c>
-      <c r="F16" s="25">
+      <c r="F16" s="37">
         <v>44615</v>
       </c>
-      <c r="G16" s="25">
+      <c r="G16" s="37">
         <v>44617</v>
       </c>
     </row>
@@ -7163,16 +7471,16 @@
       <c r="C17" s="8" t="s">
         <v>306</v>
       </c>
-      <c r="D17" s="25">
+      <c r="D17" s="37">
         <v>44627</v>
       </c>
-      <c r="E17" s="25">
+      <c r="E17" s="37">
         <v>44629</v>
       </c>
-      <c r="F17" s="25">
+      <c r="F17" s="37">
         <v>44629</v>
       </c>
-      <c r="G17" s="25">
+      <c r="G17" s="37">
         <v>44628</v>
       </c>
     </row>
@@ -7186,16 +7494,16 @@
       <c r="C18" s="5" t="s">
         <v>303</v>
       </c>
-      <c r="D18" s="26">
+      <c r="D18" s="38">
         <v>44601</v>
       </c>
-      <c r="E18" s="26">
+      <c r="E18" s="38">
         <v>44600</v>
       </c>
-      <c r="F18" s="26">
+      <c r="F18" s="38">
         <v>44600</v>
       </c>
-      <c r="G18" s="26">
+      <c r="G18" s="38">
         <v>44601</v>
       </c>
     </row>
@@ -7209,16 +7517,16 @@
       <c r="C19" s="5" t="s">
         <v>304</v>
       </c>
-      <c r="D19" s="26">
+      <c r="D19" s="38">
         <v>44614</v>
       </c>
-      <c r="E19" s="26">
+      <c r="E19" s="38">
         <v>44615</v>
       </c>
-      <c r="F19" s="26">
+      <c r="F19" s="38">
         <v>44615</v>
       </c>
-      <c r="G19" s="26">
+      <c r="G19" s="38">
         <v>44617</v>
       </c>
     </row>
@@ -7232,16 +7540,16 @@
       <c r="C20" s="8" t="s">
         <v>303</v>
       </c>
-      <c r="D20" s="25">
+      <c r="D20" s="37">
         <v>44610</v>
       </c>
-      <c r="E20" s="25">
+      <c r="E20" s="37">
         <v>44609</v>
       </c>
-      <c r="F20" s="25">
+      <c r="F20" s="37">
         <v>44609</v>
       </c>
-      <c r="G20" s="25">
+      <c r="G20" s="37">
         <v>44610</v>
       </c>
     </row>
@@ -7255,16 +7563,16 @@
       <c r="C21" s="8" t="s">
         <v>304</v>
       </c>
-      <c r="D21" s="25">
+      <c r="D21" s="37">
         <v>44623</v>
       </c>
-      <c r="E21" s="25">
+      <c r="E21" s="37">
         <v>44622</v>
       </c>
-      <c r="F21" s="25">
+      <c r="F21" s="37">
         <v>44622</v>
       </c>
-      <c r="G21" s="25">
+      <c r="G21" s="37">
         <v>44623</v>
       </c>
     </row>
@@ -7278,16 +7586,16 @@
       <c r="C22" s="8" t="s">
         <v>305</v>
       </c>
-      <c r="D22" s="25">
+      <c r="D22" s="37">
         <v>44638</v>
       </c>
-      <c r="E22" s="25">
+      <c r="E22" s="37">
         <v>44637</v>
       </c>
-      <c r="F22" s="25">
+      <c r="F22" s="37">
         <v>44637</v>
       </c>
-      <c r="G22" s="25">
+      <c r="G22" s="37">
         <v>44636</v>
       </c>
     </row>
@@ -7301,16 +7609,16 @@
       <c r="C23" s="8" t="s">
         <v>306</v>
       </c>
-      <c r="D23" s="25">
+      <c r="D23" s="37">
         <v>44652</v>
       </c>
-      <c r="E23" s="25">
+      <c r="E23" s="37">
         <v>44651</v>
       </c>
-      <c r="F23" s="25">
+      <c r="F23" s="37">
         <v>44651</v>
       </c>
-      <c r="G23" s="25">
+      <c r="G23" s="37">
         <v>44650</v>
       </c>
     </row>
@@ -7324,16 +7632,16 @@
       <c r="C24" s="5" t="s">
         <v>303</v>
       </c>
-      <c r="D24" s="26">
+      <c r="D24" s="38">
         <v>44616</v>
       </c>
-      <c r="E24" s="26">
+      <c r="E24" s="38">
         <v>44616</v>
       </c>
-      <c r="F24" s="26">
+      <c r="F24" s="38">
         <v>44616</v>
       </c>
-      <c r="G24" s="26">
+      <c r="G24" s="38">
         <v>44617</v>
       </c>
     </row>
@@ -7347,16 +7655,16 @@
       <c r="C25" s="5" t="s">
         <v>304</v>
       </c>
-      <c r="D25" s="26">
+      <c r="D25" s="38">
         <v>44630</v>
       </c>
-      <c r="E25" s="26">
+      <c r="E25" s="38">
         <v>44629</v>
       </c>
-      <c r="F25" s="26">
+      <c r="F25" s="38">
         <v>44629</v>
       </c>
-      <c r="G25" s="26">
+      <c r="G25" s="38">
         <v>44628</v>
       </c>
     </row>

</xml_diff>